<commit_message>
02.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -104,10 +104,10 @@
     <t>Rahinul Islam</t>
   </si>
   <si>
-    <t>Date: 01.10.19</t>
+    <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t xml:space="preserve">                                                                          </t>
+    <t>Date: 02.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="A4" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>3</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>123</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>3000</v>
+        <v>123000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>267</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>261</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>133500</v>
+        <v>130500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>529</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>78</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>52900</v>
+        <v>7800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>8</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>49</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>2450</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>8</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>5</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>4</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>115</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>40</v>
+        <v>1150</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>190000</v>
+        <v>265000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
-        <v>26</v>
-      </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="A31" s="56" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>3</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>123</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>3000</v>
+        <v>123000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>267</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>261</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>133500</v>
+        <v>130500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>529</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>78</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>52900</v>
+        <v>7800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>8</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>49</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>2450</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>8</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>5</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>160</v>
+        <v>100</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>4</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>115</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>40</v>
+        <v>1150</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>190000</v>
+        <v>265000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
-        <v>27</v>
-      </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="H46" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,6 +3602,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3616,26 +3636,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,6 +4389,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,30 +4429,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,16 +5167,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5189,24 +5197,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,12 +5859,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5877,32 +5903,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,12 +6343,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6365,23 +6382,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
03.10.19 Today Sales Detauls
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 02.10.19</t>
+    <t>Date: 03.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,83 +494,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,15 +588,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,6 +601,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,12 +628,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,14 +2805,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2825,24 +2835,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H46" sqref="A1:J46"/>
+    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
+      <selection sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>123</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>120</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>123000</v>
+        <v>120000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>261</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>85</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>130500</v>
+        <v>42500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>78</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>75</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>7800</v>
+        <v>7500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>49</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>220</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>2450</v>
+        <v>11000</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,11 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>5</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3050,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
-        <v>115</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1150</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3064,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>265000</v>
+        <v>181000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3123,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3163,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3175,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3264,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3326,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3344,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>123</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>120</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>123000</v>
+        <v>120000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3363,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>261</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>85</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>130500</v>
+        <v>42500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3382,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>78</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>75</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>7800</v>
+        <v>7500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3401,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>49</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>220</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>2450</v>
+        <v>11000</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3420,11 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>5</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53"/>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3437,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
-        <v>115</v>
-      </c>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1150</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3451,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>265000</v>
+        <v>181000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3510,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3550,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53" t="s">
+      <c r="H46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3564,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,26 +3594,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3636,6 +3608,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3658,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3724,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3742,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3761,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3780,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3799,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3818,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3837,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3851,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3901,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4045,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4107,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4125,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4144,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4163,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4182,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4201,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4220,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4234,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4284,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,30 +4381,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4429,6 +4397,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4452,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4518,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4536,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4555,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4574,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4593,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4610,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4627,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4641,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4691,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4831,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4893,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4911,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4930,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4949,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4968,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4985,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5002,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5016,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5066,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,6 +5159,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5179,34 +5199,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5223,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5291,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5303,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5315,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5327,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5339,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5351,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5362,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5407,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5462,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5551,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5615,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5633,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5652,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5671,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5690,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5707,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5724,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5790,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,20 +5851,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5885,24 +5887,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5920,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6101,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6119,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6136,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6155,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6172,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6191,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6208,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6274,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,29 +6335,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6382,6 +6357,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
06.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 05.10.19</t>
+    <t>Date: 06.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,83 +494,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,15 +588,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,6 +601,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,12 +628,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,14 +2805,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2825,24 +2835,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="M30" sqref="M30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>134</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>50</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>134000</v>
+        <v>50000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>161</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>136</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>80500</v>
+        <v>68000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>400</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>75</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>40000</v>
+        <v>7500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>8</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>26</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>155</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>35</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>3100</v>
+        <v>700</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,11 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>50</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3066,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>258000</v>
+        <v>128000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3125,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3165,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3177,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3266,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3328,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3346,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>134</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>50</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>134000</v>
+        <v>50000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3365,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>161</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>136</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>80500</v>
+        <v>68000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3384,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>400</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>75</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>40000</v>
+        <v>7500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3403,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>8</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>26</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>400</v>
+        <v>1300</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3422,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>155</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>35</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>3100</v>
+        <v>700</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3441,11 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>50</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>500</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3455,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>258000</v>
+        <v>128000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3514,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3554,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53" t="s">
+      <c r="H46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3568,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3598,26 +3602,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3632,6 +3616,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3662,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3728,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3746,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3765,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3784,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3803,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3822,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3841,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3855,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3905,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4049,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4111,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4129,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4148,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4167,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4186,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4205,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4224,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4238,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4288,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4385,30 +4389,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4425,6 +4405,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4456,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4522,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4540,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4559,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4578,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4597,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4614,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4631,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4645,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4695,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4835,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4897,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4915,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4934,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4953,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4972,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4989,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5006,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5020,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5070,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5163,6 +5167,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5175,34 +5207,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5227,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5295,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5307,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5319,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5331,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5343,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5355,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5366,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5411,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5466,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5555,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5619,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5637,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5656,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5675,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5694,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5711,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5728,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5794,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5855,20 +5859,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5881,24 +5895,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5924,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6105,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6123,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6140,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6159,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6176,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6195,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6212,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6278,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6339,29 +6343,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6378,6 +6365,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
07.10.19 today Saels Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 06.10.19</t>
+    <t>Date: 07.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>50</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>44</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>50000</v>
+        <v>44000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>136</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>106</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>68000</v>
+        <v>53000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>75</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>103</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>7500</v>
+        <v>10300</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>26</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>4</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>1300</v>
+        <v>200</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>35</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>25</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>50</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3066,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>128000</v>
+        <v>108000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3125,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3165,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3177,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3266,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3328,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3346,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>50</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>44</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>50000</v>
+        <v>44000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3365,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>136</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>106</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>68000</v>
+        <v>53000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3384,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>75</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>103</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>7500</v>
+        <v>10300</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3403,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>26</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>4</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>1300</v>
+        <v>200</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3422,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>35</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>25</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>700</v>
+        <v>500</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3441,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>50</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>500</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3455,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>128000</v>
+        <v>108000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3514,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3554,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3568,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,6 +3598,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3616,26 +3632,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3662,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3728,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3746,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3765,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3784,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3803,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3822,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3841,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3855,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3905,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4049,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4111,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4129,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4148,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4167,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4186,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4205,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4224,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4238,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4288,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,6 +4385,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,30 +4425,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4456,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4522,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4540,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4559,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4578,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4597,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4614,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4631,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4645,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4695,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4835,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4897,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4915,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4934,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4953,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4972,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4989,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5006,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5020,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5070,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,16 +5163,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5189,24 +5193,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5227,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5295,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5307,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5319,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5331,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5343,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5355,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5366,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5411,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5466,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5555,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5619,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5637,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5656,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5675,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5694,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5711,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5728,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5794,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,12 +5855,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5877,32 +5899,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5924,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6105,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6123,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6140,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6159,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6176,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6195,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6212,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6278,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,12 +6339,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6365,23 +6378,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
08.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 07.10.19</t>
+    <t>Date: 08.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,83 +494,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,15 +588,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,6 +601,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,12 +628,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,14 +2805,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2825,24 +2835,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>44</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>45</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>44000</v>
+        <v>45000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>106</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>146</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>53000</v>
+        <v>73000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>103</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>311</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>10300</v>
+        <v>31100</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>4</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>82</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>200</v>
+        <v>4100</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>25</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>84</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>500</v>
+        <v>1680</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,11 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58"/>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>12</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3066,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>108000</v>
+        <v>155000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3125,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3165,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3177,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3266,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3328,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3346,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>44</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>45</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>44000</v>
+        <v>45000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3365,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>106</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>146</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>53000</v>
+        <v>73000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3384,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>103</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>311</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>10300</v>
+        <v>31100</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3403,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>4</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>82</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>200</v>
+        <v>4100</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3422,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>25</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>84</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>500</v>
+        <v>1680</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3441,11 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>12</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3455,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>108000</v>
+        <v>155000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3514,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3554,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53" t="s">
+      <c r="H46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3568,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3598,26 +3602,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3632,6 +3616,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3662,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3728,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3746,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3765,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3784,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3803,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3822,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3841,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3855,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3905,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4049,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4111,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4129,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4148,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4167,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4186,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4205,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4224,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4238,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4288,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4385,30 +4389,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4425,6 +4405,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4456,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4522,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4540,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4559,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4578,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4597,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4614,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4631,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4645,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4695,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4835,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4897,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4915,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4934,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4953,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4972,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4989,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5006,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5020,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5070,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5163,6 +5167,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5175,34 +5207,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5227,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5295,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5307,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5319,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5331,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5343,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5355,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5366,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5411,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5466,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5555,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5619,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5637,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5656,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5675,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5694,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5711,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5728,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5794,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5855,20 +5859,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5881,24 +5895,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5924,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6105,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6123,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6140,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6159,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6176,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6195,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6212,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6278,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6339,29 +6343,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6378,6 +6365,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
09.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 08.10.19</t>
+    <t>Date: 09.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2854,7 +2854,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>45</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>40</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>45000</v>
+        <v>40000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>146</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>225</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>73000</v>
+        <v>112500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>311</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>208</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>31100</v>
+        <v>20800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>82</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>129</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>4100</v>
+        <v>6450</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>84</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>9</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>1680</v>
+        <v>180</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>12</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>7</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>155000</v>
+        <v>180000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>45</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>40</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>45000</v>
+        <v>40000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>146</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>225</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>73000</v>
+        <v>112500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>311</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>208</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>31100</v>
+        <v>20800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>82</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>129</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>4100</v>
+        <v>6450</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>84</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>9</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>1680</v>
+        <v>180</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>12</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>7</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>120</v>
+        <v>70</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>155000</v>
+        <v>180000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,6 +3602,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3616,26 +3636,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,6 +4389,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,30 +4429,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,16 +5167,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5189,24 +5197,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,12 +5859,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5877,32 +5903,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,12 +6343,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6365,23 +6382,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
10.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 09.10.19</t>
+    <t>Date: 10.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,83 +494,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,15 +588,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,6 +601,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,12 +628,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,14 +2805,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2825,24 +2835,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>40</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>45</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>40000</v>
+        <v>45000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>225</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>107</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>112500</v>
+        <v>53500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>208</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>105</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>20800</v>
+        <v>10500</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,11 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>129</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>6450</v>
+        <v>0</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3031,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>9</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>100</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>180</v>
+        <v>2000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3050,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
-        <v>7</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53"/>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3064,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>180000</v>
+        <v>111000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3123,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3163,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3175,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3264,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3326,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3344,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>40</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>45</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>40000</v>
+        <v>45000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3363,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>225</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>107</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>112500</v>
+        <v>53500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3382,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>208</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>105</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>20800</v>
+        <v>10500</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3401,11 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>129</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53"/>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>6450</v>
+        <v>0</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3418,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>9</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>100</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>180</v>
+        <v>2000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3437,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
-        <v>7</v>
-      </c>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53"/>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>70</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3451,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>180000</v>
+        <v>111000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3510,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3550,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53" t="s">
+      <c r="H46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3564,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,26 +3594,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3636,6 +3608,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3658,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3724,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3742,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3761,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3780,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3799,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3818,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3837,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3851,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3901,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4045,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4107,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4125,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4144,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4163,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4182,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4201,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4220,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4234,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4284,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,30 +4381,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4429,6 +4397,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4452,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4518,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4536,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4555,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4574,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4593,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4610,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4627,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4641,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4691,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4831,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4893,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4911,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4930,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4949,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4968,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4985,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5002,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5016,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5066,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,6 +5159,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5179,34 +5199,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5223,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5291,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5303,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5315,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5327,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5339,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5351,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5362,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5407,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5462,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5551,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5615,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5633,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5652,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5671,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5690,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5707,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5724,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5790,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,20 +5851,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5885,24 +5887,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5920,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6101,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6119,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6136,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6155,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6172,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6191,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6208,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6274,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,29 +6335,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6382,6 +6357,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
12.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 10.10.19</t>
+    <t>Date: 12.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>45</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>38</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>45000</v>
+        <v>38000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>107</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>133</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>53500</v>
+        <v>66500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>105</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>398</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>10500</v>
+        <v>39800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,11 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53"/>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>107</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>5350</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3031,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>100</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>7</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>2000</v>
+        <v>140</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3050,11 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53"/>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>21</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3064,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>111000</v>
+        <v>150000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3123,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3163,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3175,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3264,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3326,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3344,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>45</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>38</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>45000</v>
+        <v>38000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3363,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>107</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>133</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>53500</v>
+        <v>66500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3382,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>105</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>398</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>10500</v>
+        <v>39800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3401,11 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53"/>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>107</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>5350</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3418,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>100</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>7</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>2000</v>
+        <v>140</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3437,11 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53"/>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>21</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>210</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3451,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>111000</v>
+        <v>150000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3510,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3550,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3564,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3594,6 +3602,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3608,26 +3636,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3658,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3724,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3742,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3761,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3780,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3799,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3818,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3837,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3851,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3901,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4045,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4107,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4125,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4144,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4163,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4182,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4201,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4220,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4234,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4284,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4381,6 +4389,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4397,30 +4429,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4452,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4518,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4536,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4555,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4574,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4593,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4610,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4627,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4641,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4691,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4831,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4893,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4911,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4930,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4949,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4968,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4985,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5002,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5016,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5066,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5159,16 +5167,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5181,24 +5197,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5223,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5291,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5303,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5315,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5327,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5339,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5351,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5362,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5407,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5462,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5551,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5615,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5633,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5652,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5671,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5690,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5707,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5724,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5790,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5851,12 +5859,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5869,32 +5903,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5920,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6101,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6119,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6136,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6155,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6172,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6191,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6208,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6274,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6335,12 +6343,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6357,23 +6382,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
17.10.19 Today Sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 15.10.19</t>
+    <t>Date: 17.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2855,7 +2855,7 @@
   <dimension ref="A1:K49"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K47" sqref="A1:K47"/>
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>33</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>39</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>33000</v>
+        <v>39000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>139</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>154</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>69500</v>
+        <v>77000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>137</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>428</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>13700</v>
+        <v>42800</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>148</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>4</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>7400</v>
+        <v>200</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>15</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>200</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>300</v>
+        <v>4000</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,11 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>110</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58"/>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3066,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>125000</v>
+        <v>163000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3125,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3165,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3177,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3266,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3328,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3346,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>33</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>39</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>33000</v>
+        <v>39000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3365,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>139</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>154</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>69500</v>
+        <v>77000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3384,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>137</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>428</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>13700</v>
+        <v>42800</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3403,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>148</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>4</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>7400</v>
+        <v>200</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3422,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>15</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>200</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>300</v>
+        <v>4000</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3441,11 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>110</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58"/>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1100</v>
+        <v>0</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3455,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>125000</v>
+        <v>163000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3514,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3554,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3568,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,6 +3598,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3616,26 +3632,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3662,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3728,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3746,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3765,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3784,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3803,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3822,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3841,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3855,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3905,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4049,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4111,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4129,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4148,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4167,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4186,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4205,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4224,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4238,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4288,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,6 +4385,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,30 +4425,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4456,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4522,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4540,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4559,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4578,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4597,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4614,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4631,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4645,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4695,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4835,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4897,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4915,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4934,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4953,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4972,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4989,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5006,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5020,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5070,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,16 +5163,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5189,24 +5193,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5227,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5295,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5307,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5319,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5331,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5343,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5355,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5366,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5411,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5466,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5555,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5619,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5637,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5656,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5675,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5694,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5711,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5728,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5794,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,12 +5855,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5877,32 +5899,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5924,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6105,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6123,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6140,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6159,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6176,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6195,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6212,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6278,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,12 +6339,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6365,23 +6378,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
20.10.19 Today sales Details
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 19.10.19</t>
+    <t>Date: 20.10.19</t>
   </si>
 </sst>
 </file>
@@ -2854,8 +2854,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection sqref="A1:J46"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H46" sqref="A1:J46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2958,12 +2958,12 @@
         <v>1000</v>
       </c>
       <c r="E6" s="58">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>56000</v>
+        <v>22000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2977,12 +2977,12 @@
         <v>500</v>
       </c>
       <c r="E7" s="58">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>47000</v>
+        <v>100000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2996,12 +2996,12 @@
         <v>100</v>
       </c>
       <c r="E8" s="58">
-        <v>240</v>
+        <v>324</v>
       </c>
       <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>24000</v>
+        <v>32400</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3015,12 +3015,12 @@
         <v>50</v>
       </c>
       <c r="E9" s="58">
-        <v>100</v>
+        <v>302</v>
       </c>
       <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>5000</v>
+        <v>15100</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,11 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58"/>
+      <c r="E10" s="58">
+        <v>75</v>
+      </c>
       <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3050,11 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58"/>
+      <c r="E11" s="58">
+        <v>100</v>
+      </c>
       <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3071,7 +3075,7 @@
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>132000</v>
+        <v>172000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3345,12 +3349,12 @@
         <v>1000</v>
       </c>
       <c r="E33" s="58">
-        <v>56</v>
+        <v>22</v>
       </c>
       <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>56000</v>
+        <v>22000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3364,12 +3368,12 @@
         <v>500</v>
       </c>
       <c r="E34" s="58">
-        <v>94</v>
+        <v>200</v>
       </c>
       <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>47000</v>
+        <v>100000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3383,12 +3387,12 @@
         <v>100</v>
       </c>
       <c r="E35" s="58">
-        <v>240</v>
+        <v>324</v>
       </c>
       <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>24000</v>
+        <v>32400</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3402,12 +3406,12 @@
         <v>50</v>
       </c>
       <c r="E36" s="58">
-        <v>100</v>
+        <v>302</v>
       </c>
       <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>5000</v>
+        <v>15100</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3420,11 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58"/>
+      <c r="E37" s="58">
+        <v>75</v>
+      </c>
       <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>0</v>
+        <v>1500</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3437,11 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58"/>
+      <c r="E38" s="58">
+        <v>100</v>
+      </c>
       <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>0</v>
+        <v>1000</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3458,7 +3466,7 @@
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>132000</v>
+        <v>172000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>

</xml_diff>

<commit_message>
21.10.19 Today Sales Detsils
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 20.10.19</t>
+    <t>Date: 21.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,83 +494,86 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -585,15 +588,12 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,6 +601,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -622,12 +628,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>50</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>16</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>151</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>58</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>50</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>116</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>151</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>58</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="46" t="s">
+      <c r="D38" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="47"/>
+      <c r="E38" s="38"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,14 +2805,24 @@
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E37:F37"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A27:J27"/>
@@ -2825,24 +2835,14 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="54" t="s">
+      <c r="A1" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="54"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
-      <c r="G1" s="54"/>
-      <c r="H1" s="54"/>
-      <c r="I1" s="54"/>
-      <c r="J1" s="54"/>
+      <c r="B1" s="49"/>
+      <c r="C1" s="49"/>
+      <c r="D1" s="49"/>
+      <c r="E1" s="49"/>
+      <c r="F1" s="49"/>
+      <c r="G1" s="49"/>
+      <c r="H1" s="49"/>
+      <c r="I1" s="49"/>
+      <c r="J1" s="49"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="55" t="s">
+      <c r="A2" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="55"/>
-      <c r="D2" s="55"/>
-      <c r="E2" s="55"/>
-      <c r="F2" s="55"/>
-      <c r="G2" s="55"/>
-      <c r="H2" s="55"/>
-      <c r="I2" s="55"/>
-      <c r="J2" s="55"/>
+      <c r="B2" s="50"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="55" t="s">
+      <c r="A3" s="50" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="55"/>
-      <c r="D3" s="55"/>
-      <c r="E3" s="55"/>
-      <c r="F3" s="55"/>
-      <c r="G3" s="55"/>
-      <c r="H3" s="55"/>
-      <c r="I3" s="55"/>
-      <c r="J3" s="55"/>
+      <c r="B3" s="50"/>
+      <c r="C3" s="50"/>
+      <c r="D3" s="50"/>
+      <c r="E3" s="50"/>
+      <c r="F3" s="50"/>
+      <c r="G3" s="50"/>
+      <c r="H3" s="50"/>
+      <c r="I3" s="50"/>
+      <c r="J3" s="50"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="56" t="s">
+      <c r="A4" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="56"/>
-      <c r="C4" s="56"/>
-      <c r="D4" s="56"/>
-      <c r="E4" s="56"/>
-      <c r="F4" s="56"/>
-      <c r="G4" s="56"/>
-      <c r="H4" s="56"/>
-      <c r="I4" s="56"/>
-      <c r="J4" s="56"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="51"/>
+      <c r="D4" s="51"/>
+      <c r="E4" s="51"/>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="51"/>
+      <c r="J4" s="51"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="57" t="s">
+      <c r="E5" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="57"/>
+      <c r="F5" s="52"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="58">
-        <v>22</v>
-      </c>
-      <c r="F6" s="58"/>
+      <c r="E6" s="53">
+        <v>35</v>
+      </c>
+      <c r="F6" s="53"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>22000</v>
+        <v>35000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="58">
-        <v>200</v>
-      </c>
-      <c r="F7" s="58"/>
+      <c r="E7" s="53">
+        <v>237</v>
+      </c>
+      <c r="F7" s="53"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>100000</v>
+        <v>118500</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="58">
-        <v>324</v>
-      </c>
-      <c r="F8" s="58"/>
+      <c r="E8" s="53">
+        <v>77</v>
+      </c>
+      <c r="F8" s="53"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>32400</v>
+        <v>7700</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="58">
-        <v>302</v>
-      </c>
-      <c r="F9" s="58"/>
+      <c r="E9" s="53">
+        <v>9</v>
+      </c>
+      <c r="F9" s="53"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>15100</v>
+        <v>450</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="58">
-        <v>75</v>
-      </c>
-      <c r="F10" s="58"/>
+      <c r="E10" s="53">
+        <v>14</v>
+      </c>
+      <c r="F10" s="53"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>1500</v>
+        <v>280</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="58">
-        <v>100</v>
-      </c>
-      <c r="F11" s="58"/>
+      <c r="E11" s="53">
+        <v>107</v>
+      </c>
+      <c r="F11" s="53"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1000</v>
+        <v>1070</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="61" t="s">
+      <c r="D12" s="55" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="61"/>
+      <c r="E12" s="55"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>172000</v>
+        <v>163000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="51" t="s">
+      <c r="H16" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="51"/>
-      <c r="J16" s="51"/>
+      <c r="I16" s="54"/>
+      <c r="J16" s="54"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="51"/>
+      <c r="D17" s="54"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="51"/>
-      <c r="I17" s="51"/>
-      <c r="J17" s="51"/>
+      <c r="H17" s="54"/>
+      <c r="I17" s="54"/>
+      <c r="J17" s="54"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="51"/>
+      <c r="D18" s="54"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="51"/>
-      <c r="I18" s="51"/>
-      <c r="J18" s="51"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="53"/>
-      <c r="I19" s="53"/>
-      <c r="J19" s="53"/>
+      <c r="H19" s="56"/>
+      <c r="I19" s="56"/>
+      <c r="J19" s="56"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="49"/>
-      <c r="I20" s="50"/>
-      <c r="J20" s="50"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="58"/>
+      <c r="J20" s="58"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="54" t="s">
+      <c r="A28" s="49" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="54"/>
-      <c r="C28" s="54"/>
-      <c r="D28" s="54"/>
-      <c r="E28" s="54"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="54"/>
-      <c r="H28" s="54"/>
-      <c r="I28" s="54"/>
-      <c r="J28" s="54"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="49"/>
+      <c r="E28" s="49"/>
+      <c r="F28" s="49"/>
+      <c r="G28" s="49"/>
+      <c r="H28" s="49"/>
+      <c r="I28" s="49"/>
+      <c r="J28" s="49"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="55" t="s">
+      <c r="A29" s="50" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="55"/>
-      <c r="C29" s="55"/>
-      <c r="D29" s="55"/>
-      <c r="E29" s="55"/>
-      <c r="F29" s="55"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="55"/>
-      <c r="I29" s="55"/>
-      <c r="J29" s="55"/>
+      <c r="B29" s="50"/>
+      <c r="C29" s="50"/>
+      <c r="D29" s="50"/>
+      <c r="E29" s="50"/>
+      <c r="F29" s="50"/>
+      <c r="G29" s="50"/>
+      <c r="H29" s="50"/>
+      <c r="I29" s="50"/>
+      <c r="J29" s="50"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="56" t="s">
+      <c r="A30" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="56"/>
-      <c r="C30" s="56"/>
-      <c r="D30" s="56"/>
-      <c r="E30" s="56"/>
-      <c r="F30" s="56"/>
-      <c r="G30" s="56"/>
-      <c r="H30" s="56"/>
-      <c r="I30" s="56"/>
-      <c r="J30" s="56"/>
+      <c r="B30" s="51"/>
+      <c r="C30" s="51"/>
+      <c r="D30" s="51"/>
+      <c r="E30" s="51"/>
+      <c r="F30" s="51"/>
+      <c r="G30" s="51"/>
+      <c r="H30" s="51"/>
+      <c r="I30" s="51"/>
+      <c r="J30" s="51"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="56" t="s">
+      <c r="A31" s="51" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="56"/>
-      <c r="C31" s="56"/>
-      <c r="D31" s="56"/>
-      <c r="E31" s="56"/>
-      <c r="F31" s="56"/>
-      <c r="G31" s="56"/>
-      <c r="H31" s="56"/>
-      <c r="I31" s="56"/>
-      <c r="J31" s="56"/>
+      <c r="B31" s="51"/>
+      <c r="C31" s="51"/>
+      <c r="D31" s="51"/>
+      <c r="E31" s="51"/>
+      <c r="F31" s="51"/>
+      <c r="G31" s="51"/>
+      <c r="H31" s="51"/>
+      <c r="I31" s="51"/>
+      <c r="J31" s="51"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="57" t="s">
+      <c r="E32" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="57"/>
+      <c r="F32" s="52"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="58">
-        <v>22</v>
-      </c>
-      <c r="F33" s="58"/>
+      <c r="E33" s="53">
+        <v>35</v>
+      </c>
+      <c r="F33" s="53"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>22000</v>
+        <v>35000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="58">
-        <v>200</v>
-      </c>
-      <c r="F34" s="58"/>
+      <c r="E34" s="53">
+        <v>237</v>
+      </c>
+      <c r="F34" s="53"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>100000</v>
+        <v>118500</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="58">
-        <v>324</v>
-      </c>
-      <c r="F35" s="58"/>
+      <c r="E35" s="53">
+        <v>77</v>
+      </c>
+      <c r="F35" s="53"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>32400</v>
+        <v>7700</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="58">
-        <v>302</v>
-      </c>
-      <c r="F36" s="58"/>
+      <c r="E36" s="53">
+        <v>9</v>
+      </c>
+      <c r="F36" s="53"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>15100</v>
+        <v>450</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="58">
-        <v>75</v>
-      </c>
-      <c r="F37" s="58"/>
+      <c r="E37" s="53">
+        <v>14</v>
+      </c>
+      <c r="F37" s="53"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>1500</v>
+        <v>280</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="58">
-        <v>100</v>
-      </c>
-      <c r="F38" s="58"/>
+      <c r="E38" s="53">
+        <v>107</v>
+      </c>
+      <c r="F38" s="53"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1000</v>
+        <v>1070</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="59" t="s">
+      <c r="D39" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="60"/>
+      <c r="E39" s="61"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>172000</v>
+        <v>163000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="51" t="s">
+      <c r="H43" s="54" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="51"/>
-      <c r="J43" s="51"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="54"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="52"/>
+      <c r="D44" s="59"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="52"/>
-      <c r="I44" s="52"/>
-      <c r="J44" s="52"/>
+      <c r="H44" s="59"/>
+      <c r="I44" s="59"/>
+      <c r="J44" s="59"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="52"/>
+      <c r="D45" s="59"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="52"/>
-      <c r="I45" s="52"/>
-      <c r="J45" s="52"/>
+      <c r="H45" s="59"/>
+      <c r="I45" s="59"/>
+      <c r="J45" s="59"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="53" t="s">
+      <c r="H46" s="56" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="53"/>
-      <c r="J46" s="53"/>
+      <c r="I46" s="56"/>
+      <c r="J46" s="56"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,26 +3602,6 @@
     </row>
   </sheetData>
   <mergeCells count="34">
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3636,6 +3616,26 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>68</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>135</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>53</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39">
+      <c r="E9" s="41">
         <v>2</v>
       </c>
-      <c r="F9" s="39"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39">
+      <c r="E10" s="41">
         <v>5</v>
       </c>
-      <c r="F10" s="39"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41" t="s">
+      <c r="A19" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="41"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="62" t="s">
+      <c r="A20" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="63"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="66" t="s">
+      <c r="E31" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="62"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="65">
+      <c r="E32" s="66">
         <v>68</v>
       </c>
-      <c r="F32" s="65"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="65">
+      <c r="E33" s="66">
         <v>135</v>
       </c>
-      <c r="F33" s="65"/>
+      <c r="F33" s="66"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="65">
+      <c r="E34" s="66">
         <v>53</v>
       </c>
-      <c r="F34" s="65"/>
+      <c r="F34" s="66"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="65">
+      <c r="E35" s="66">
         <v>2</v>
       </c>
-      <c r="F35" s="65"/>
+      <c r="F35" s="66"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="65">
+      <c r="E36" s="66">
         <v>5</v>
       </c>
-      <c r="F36" s="65"/>
+      <c r="F36" s="66"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="64" t="s">
+      <c r="D38" s="65" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="64"/>
+      <c r="E38" s="65"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41" t="s">
+      <c r="A45" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="41"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63" t="s">
+      <c r="A46" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="63"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,30 +4389,6 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4429,6 +4405,30 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="37" t="s">
+      <c r="A3" s="43" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="38" t="s">
+      <c r="A4" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="35"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="39">
+      <c r="E6" s="41">
         <v>44</v>
       </c>
-      <c r="F6" s="39"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="39">
+      <c r="E7" s="41">
         <v>118</v>
       </c>
-      <c r="F7" s="39"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="39">
+      <c r="E8" s="41">
         <v>510</v>
       </c>
-      <c r="F8" s="39"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35" t="s">
+      <c r="D12" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="35"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="40" t="s">
+      <c r="A16" s="47" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="40"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40" t="s">
+      <c r="H16" s="47" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42" t="s">
+      <c r="H19" s="48" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="68"/>
-      <c r="B20" s="68"/>
+      <c r="A20" s="67"/>
+      <c r="B20" s="67"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43" t="s">
+      <c r="H20" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="36" t="s">
+      <c r="A27" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="36"/>
-      <c r="C27" s="36"/>
-      <c r="D27" s="36"/>
-      <c r="E27" s="36"/>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36"/>
-      <c r="H27" s="36"/>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="B27" s="42"/>
+      <c r="C27" s="42"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="42"/>
+      <c r="G27" s="42"/>
+      <c r="H27" s="42"/>
+      <c r="I27" s="42"/>
+      <c r="J27" s="42"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="37" t="s">
+      <c r="A28" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="37"/>
-      <c r="C28" s="37"/>
-      <c r="D28" s="37"/>
-      <c r="E28" s="37"/>
-      <c r="F28" s="37"/>
-      <c r="G28" s="37"/>
-      <c r="H28" s="37"/>
-      <c r="I28" s="37"/>
-      <c r="J28" s="37"/>
+      <c r="B28" s="43"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
+      <c r="G28" s="43"/>
+      <c r="H28" s="43"/>
+      <c r="I28" s="43"/>
+      <c r="J28" s="43"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="45"/>
-      <c r="C29" s="45"/>
-      <c r="D29" s="45"/>
-      <c r="E29" s="45"/>
-      <c r="F29" s="45"/>
-      <c r="G29" s="45"/>
-      <c r="H29" s="45"/>
-      <c r="I29" s="45"/>
-      <c r="J29" s="45"/>
+      <c r="B29" s="44"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="44"/>
+      <c r="E29" s="44"/>
+      <c r="F29" s="44"/>
+      <c r="G29" s="44"/>
+      <c r="H29" s="44"/>
+      <c r="I29" s="44"/>
+      <c r="J29" s="44"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="38" t="s">
+      <c r="A30" s="45" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="38"/>
-      <c r="C30" s="38"/>
-      <c r="D30" s="38"/>
-      <c r="E30" s="38"/>
-      <c r="F30" s="38"/>
-      <c r="G30" s="38"/>
-      <c r="H30" s="38"/>
-      <c r="I30" s="38"/>
-      <c r="J30" s="38"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="35" t="s">
+      <c r="E31" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="35"/>
+      <c r="F31" s="46"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="39">
+      <c r="E32" s="41">
         <v>44</v>
       </c>
-      <c r="F32" s="39"/>
+      <c r="F32" s="41"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>118</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>510</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="39"/>
-      <c r="F35" s="39"/>
+      <c r="E35" s="41"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="39"/>
-      <c r="F37" s="39"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="41"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="67" t="s">
+      <c r="D38" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="67"/>
+      <c r="E38" s="68"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="48" t="s">
+      <c r="A42" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="48"/>
+      <c r="B42" s="39"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="48" t="s">
+      <c r="H42" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="48"/>
-      <c r="J42" s="48"/>
+      <c r="I42" s="39"/>
+      <c r="J42" s="39"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="41"/>
-      <c r="B43" s="41"/>
+      <c r="A43" s="40"/>
+      <c r="B43" s="40"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="41"/>
-      <c r="I43" s="41"/>
-      <c r="J43" s="41"/>
+      <c r="H43" s="40"/>
+      <c r="I43" s="40"/>
+      <c r="J43" s="40"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41" t="s">
+      <c r="H45" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="48"/>
-      <c r="J45" s="48"/>
+      <c r="I45" s="39"/>
+      <c r="J45" s="39"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="63"/>
-      <c r="B46" s="63"/>
+      <c r="A46" s="64"/>
+      <c r="B46" s="64"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="43" t="s">
+      <c r="H46" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="44"/>
-      <c r="J46" s="44"/>
+      <c r="I46" s="36"/>
+      <c r="J46" s="36"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,6 +5167,34 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5179,34 +5207,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="37"/>
-      <c r="B3" s="37"/>
-      <c r="C3" s="37"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="37"/>
-      <c r="F3" s="37"/>
-      <c r="G3" s="37"/>
-      <c r="H3" s="37"/>
-      <c r="I3" s="37"/>
-      <c r="J3" s="37"/>
+      <c r="A3" s="43"/>
+      <c r="B3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="43"/>
+      <c r="E3" s="43"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="43"/>
+      <c r="J3" s="43"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="38"/>
-      <c r="B4" s="38"/>
-      <c r="C4" s="38"/>
-      <c r="D4" s="38"/>
-      <c r="E4" s="38"/>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="38"/>
-      <c r="J4" s="38"/>
+      <c r="A4" s="45"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="45"/>
+      <c r="D4" s="45"/>
+      <c r="E4" s="45"/>
+      <c r="F4" s="45"/>
+      <c r="G4" s="45"/>
+      <c r="H4" s="45"/>
+      <c r="I4" s="45"/>
+      <c r="J4" s="45"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="35"/>
-      <c r="F5" s="35"/>
+      <c r="E5" s="46"/>
+      <c r="F5" s="46"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="39"/>
-      <c r="F8" s="39"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="39"/>
-      <c r="F9" s="39"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="39"/>
-      <c r="F10" s="39"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="39"/>
-      <c r="F11" s="39"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="35"/>
-      <c r="E12" s="35"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="46"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="40"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="47"/>
+      <c r="B16" s="47"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="40"/>
-      <c r="I16" s="40"/>
-      <c r="J16" s="40"/>
+      <c r="H16" s="47"/>
+      <c r="I16" s="47"/>
+      <c r="J16" s="47"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="40"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="47"/>
+      <c r="B17" s="47"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="40"/>
-      <c r="I17" s="40"/>
-      <c r="J17" s="40"/>
+      <c r="H17" s="47"/>
+      <c r="I17" s="47"/>
+      <c r="J17" s="47"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="40"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="47"/>
+      <c r="B18" s="47"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="40"/>
-      <c r="I18" s="40"/>
-      <c r="J18" s="40"/>
+      <c r="H18" s="47"/>
+      <c r="I18" s="47"/>
+      <c r="J18" s="47"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="41"/>
-      <c r="B19" s="41"/>
+      <c r="A19" s="40"/>
+      <c r="B19" s="40"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="42"/>
-      <c r="I19" s="42"/>
-      <c r="J19" s="42"/>
+      <c r="H19" s="48"/>
+      <c r="I19" s="48"/>
+      <c r="J19" s="48"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="43"/>
-      <c r="I20" s="44"/>
-      <c r="J20" s="44"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="36"/>
+      <c r="J20" s="36"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="36" t="s">
+      <c r="A28" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="36"/>
-      <c r="C28" s="36"/>
-      <c r="D28" s="36"/>
-      <c r="E28" s="36"/>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36"/>
-      <c r="H28" s="36"/>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="B28" s="42"/>
+      <c r="C28" s="42"/>
+      <c r="D28" s="42"/>
+      <c r="E28" s="42"/>
+      <c r="F28" s="42"/>
+      <c r="G28" s="42"/>
+      <c r="H28" s="42"/>
+      <c r="I28" s="42"/>
+      <c r="J28" s="42"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="37" t="s">
+      <c r="A29" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="37"/>
-      <c r="C29" s="37"/>
-      <c r="D29" s="37"/>
-      <c r="E29" s="37"/>
-      <c r="F29" s="37"/>
-      <c r="G29" s="37"/>
-      <c r="H29" s="37"/>
-      <c r="I29" s="37"/>
-      <c r="J29" s="37"/>
+      <c r="B29" s="43"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
+      <c r="G29" s="43"/>
+      <c r="H29" s="43"/>
+      <c r="I29" s="43"/>
+      <c r="J29" s="43"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="44"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="44"/>
+      <c r="E30" s="44"/>
+      <c r="F30" s="44"/>
+      <c r="G30" s="44"/>
+      <c r="H30" s="44"/>
+      <c r="I30" s="44"/>
+      <c r="J30" s="44"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="38" t="s">
+      <c r="A31" s="45" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="38"/>
-      <c r="C31" s="38"/>
-      <c r="D31" s="38"/>
-      <c r="E31" s="38"/>
-      <c r="F31" s="38"/>
-      <c r="G31" s="38"/>
-      <c r="H31" s="38"/>
-      <c r="I31" s="38"/>
-      <c r="J31" s="38"/>
+      <c r="B31" s="45"/>
+      <c r="C31" s="45"/>
+      <c r="D31" s="45"/>
+      <c r="E31" s="45"/>
+      <c r="F31" s="45"/>
+      <c r="G31" s="45"/>
+      <c r="H31" s="45"/>
+      <c r="I31" s="45"/>
+      <c r="J31" s="45"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="66" t="s">
+      <c r="E32" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="62"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="39">
+      <c r="E33" s="41">
         <v>30</v>
       </c>
-      <c r="F33" s="39"/>
+      <c r="F33" s="41"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="39">
+      <c r="E34" s="41">
         <v>35</v>
       </c>
-      <c r="F34" s="39"/>
+      <c r="F34" s="41"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="39">
+      <c r="E35" s="41">
         <v>425</v>
       </c>
-      <c r="F35" s="39"/>
+      <c r="F35" s="41"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="39"/>
-      <c r="F36" s="39"/>
+      <c r="E36" s="41"/>
+      <c r="F36" s="41"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="65"/>
-      <c r="F37" s="65"/>
+      <c r="E37" s="66"/>
+      <c r="F37" s="66"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="65">
+      <c r="E38" s="66">
         <v>100</v>
       </c>
-      <c r="F38" s="65"/>
+      <c r="F38" s="66"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="48" t="s">
+      <c r="A43" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="48"/>
+      <c r="B43" s="39"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="48" t="s">
+      <c r="H43" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="48"/>
-      <c r="J43" s="48"/>
+      <c r="I43" s="39"/>
+      <c r="J43" s="39"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="41"/>
-      <c r="B44" s="41"/>
+      <c r="A44" s="40"/>
+      <c r="B44" s="40"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="41"/>
-      <c r="I44" s="41"/>
-      <c r="J44" s="41"/>
+      <c r="H44" s="40"/>
+      <c r="I44" s="40"/>
+      <c r="J44" s="40"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="41"/>
-      <c r="B45" s="41"/>
+      <c r="A45" s="40"/>
+      <c r="B45" s="40"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="41"/>
-      <c r="I45" s="41"/>
-      <c r="J45" s="41"/>
+      <c r="H45" s="40"/>
+      <c r="I45" s="40"/>
+      <c r="J45" s="40"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="41"/>
-      <c r="B46" s="41"/>
+      <c r="A46" s="40"/>
+      <c r="B46" s="40"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="41" t="s">
+      <c r="H46" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="48"/>
-      <c r="J46" s="48"/>
+      <c r="I46" s="39"/>
+      <c r="J46" s="39"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,20 +5859,30 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="43"/>
-      <c r="I47" s="44"/>
-      <c r="J47" s="44"/>
+      <c r="H47" s="35"/>
+      <c r="I47" s="36"/>
+      <c r="J47" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="38">
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E38:F38"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="A28:J28"/>
@@ -5885,24 +5895,14 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36"/>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="36"/>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36"/>
-      <c r="J1" s="36"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
+      <c r="H1" s="42"/>
+      <c r="I1" s="42"/>
+      <c r="J1" s="42"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="37" t="s">
+      <c r="A2" s="43" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="37"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="43"/>
+      <c r="D2" s="43"/>
+      <c r="E2" s="43"/>
+      <c r="F2" s="43"/>
+      <c r="G2" s="43"/>
+      <c r="H2" s="43"/>
+      <c r="I2" s="43"/>
+      <c r="J2" s="43"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="79">
+      <c r="A5" s="80">
         <v>1</v>
       </c>
-      <c r="B5" s="71" t="s">
+      <c r="B5" s="73" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="71"/>
-      <c r="D5" s="71"/>
-      <c r="E5" s="71"/>
-      <c r="F5" s="71"/>
-      <c r="G5" s="78">
+      <c r="C5" s="73"/>
+      <c r="D5" s="73"/>
+      <c r="E5" s="73"/>
+      <c r="F5" s="73"/>
+      <c r="G5" s="71">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="79"/>
-      <c r="B6" s="71"/>
-      <c r="C6" s="71"/>
-      <c r="D6" s="71"/>
-      <c r="E6" s="71"/>
-      <c r="F6" s="71"/>
-      <c r="G6" s="78"/>
+      <c r="A6" s="80"/>
+      <c r="B6" s="73"/>
+      <c r="C6" s="73"/>
+      <c r="D6" s="73"/>
+      <c r="E6" s="73"/>
+      <c r="F6" s="73"/>
+      <c r="G6" s="71"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="79">
+      <c r="A7" s="80">
         <v>2</v>
       </c>
-      <c r="B7" s="71" t="s">
+      <c r="B7" s="73" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="71"/>
-      <c r="D7" s="71"/>
-      <c r="E7" s="71"/>
-      <c r="F7" s="71"/>
-      <c r="G7" s="78">
+      <c r="C7" s="73"/>
+      <c r="D7" s="73"/>
+      <c r="E7" s="73"/>
+      <c r="F7" s="73"/>
+      <c r="G7" s="71">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="79"/>
-      <c r="B8" s="71"/>
-      <c r="C8" s="71"/>
-      <c r="D8" s="71"/>
-      <c r="E8" s="71"/>
-      <c r="F8" s="71"/>
-      <c r="G8" s="78"/>
+      <c r="A8" s="80"/>
+      <c r="B8" s="73"/>
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="71"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="79">
+      <c r="A9" s="80">
         <v>3</v>
       </c>
-      <c r="B9" s="71" t="s">
+      <c r="B9" s="73" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="78">
+      <c r="C9" s="73"/>
+      <c r="D9" s="73"/>
+      <c r="E9" s="73"/>
+      <c r="F9" s="73"/>
+      <c r="G9" s="71">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="79"/>
-      <c r="B10" s="71"/>
-      <c r="C10" s="71"/>
-      <c r="D10" s="71"/>
-      <c r="E10" s="71"/>
-      <c r="F10" s="71"/>
-      <c r="G10" s="78"/>
+      <c r="A10" s="80"/>
+      <c r="B10" s="73"/>
+      <c r="C10" s="73"/>
+      <c r="D10" s="73"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="73"/>
+      <c r="G10" s="71"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="79">
+      <c r="A11" s="80">
         <v>4</v>
       </c>
-      <c r="B11" s="72" t="s">
+      <c r="B11" s="74" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="73"/>
-      <c r="D11" s="73"/>
-      <c r="E11" s="73"/>
-      <c r="F11" s="74"/>
-      <c r="G11" s="78">
+      <c r="C11" s="75"/>
+      <c r="D11" s="75"/>
+      <c r="E11" s="75"/>
+      <c r="F11" s="76"/>
+      <c r="G11" s="71">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="79"/>
-      <c r="B12" s="75"/>
-      <c r="C12" s="76"/>
-      <c r="D12" s="76"/>
-      <c r="E12" s="76"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="78"/>
+      <c r="A12" s="80"/>
+      <c r="B12" s="77"/>
+      <c r="C12" s="78"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="79"/>
+      <c r="G12" s="71"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="80" t="s">
+      <c r="A13" s="72" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="80"/>
-      <c r="C13" s="80"/>
-      <c r="D13" s="80"/>
-      <c r="E13" s="80"/>
-      <c r="F13" s="80"/>
-      <c r="G13" s="78">
+      <c r="B13" s="72"/>
+      <c r="C13" s="72"/>
+      <c r="D13" s="72"/>
+      <c r="E13" s="72"/>
+      <c r="F13" s="72"/>
+      <c r="G13" s="71">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="80"/>
-      <c r="B14" s="80"/>
-      <c r="C14" s="80"/>
-      <c r="D14" s="80"/>
-      <c r="E14" s="80"/>
-      <c r="F14" s="80"/>
-      <c r="G14" s="78"/>
+      <c r="A14" s="72"/>
+      <c r="B14" s="72"/>
+      <c r="C14" s="72"/>
+      <c r="D14" s="72"/>
+      <c r="E14" s="72"/>
+      <c r="F14" s="72"/>
+      <c r="G14" s="71"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="45" t="s">
+      <c r="A23" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="45"/>
-      <c r="C23" s="45"/>
-      <c r="D23" s="45"/>
-      <c r="E23" s="45"/>
-      <c r="F23" s="45"/>
-      <c r="G23" s="45"/>
-      <c r="H23" s="45"/>
-      <c r="I23" s="45"/>
-      <c r="J23" s="45"/>
+      <c r="B23" s="44"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="44"/>
+      <c r="E23" s="44"/>
+      <c r="F23" s="44"/>
+      <c r="G23" s="44"/>
+      <c r="H23" s="44"/>
+      <c r="I23" s="44"/>
+      <c r="J23" s="44"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="38"/>
-      <c r="B24" s="38"/>
-      <c r="C24" s="38"/>
-      <c r="D24" s="38"/>
-      <c r="E24" s="38"/>
-      <c r="F24" s="38"/>
-      <c r="G24" s="38"/>
-      <c r="H24" s="38"/>
-      <c r="I24" s="38"/>
-      <c r="J24" s="38"/>
+      <c r="A24" s="45"/>
+      <c r="B24" s="45"/>
+      <c r="C24" s="45"/>
+      <c r="D24" s="45"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="45"/>
+      <c r="I24" s="45"/>
+      <c r="J24" s="45"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="66" t="s">
+      <c r="E25" s="62" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="66"/>
+      <c r="F25" s="62"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="39"/>
-      <c r="F26" s="39"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="39">
+      <c r="E27" s="41">
         <v>30</v>
       </c>
-      <c r="F27" s="39"/>
+      <c r="F27" s="41"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="39"/>
-      <c r="F28" s="39"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="39">
+      <c r="E29" s="41">
         <v>5</v>
       </c>
-      <c r="F29" s="39"/>
+      <c r="F29" s="41"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="65"/>
-      <c r="F30" s="65"/>
+      <c r="E30" s="66"/>
+      <c r="F30" s="66"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="65">
+      <c r="E31" s="66">
         <v>2</v>
       </c>
-      <c r="F31" s="65"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="48" t="s">
+      <c r="A36" s="39" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="48"/>
+      <c r="B36" s="39"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="48" t="s">
+      <c r="H36" s="39" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="48"/>
-      <c r="J36" s="48"/>
+      <c r="I36" s="39"/>
+      <c r="J36" s="39"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="41"/>
-      <c r="B37" s="41"/>
+      <c r="A37" s="40"/>
+      <c r="B37" s="40"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="41"/>
-      <c r="I37" s="41"/>
-      <c r="J37" s="41"/>
+      <c r="H37" s="40"/>
+      <c r="I37" s="40"/>
+      <c r="J37" s="40"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="41"/>
-      <c r="B38" s="41"/>
+      <c r="A38" s="40"/>
+      <c r="B38" s="40"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="41"/>
-      <c r="I38" s="41"/>
-      <c r="J38" s="41"/>
+      <c r="H38" s="40"/>
+      <c r="I38" s="40"/>
+      <c r="J38" s="40"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="41"/>
-      <c r="B39" s="41"/>
+      <c r="A39" s="40"/>
+      <c r="B39" s="40"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="41" t="s">
+      <c r="H39" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="48"/>
-      <c r="J39" s="48"/>
+      <c r="I39" s="39"/>
+      <c r="J39" s="39"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,29 +6343,12 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="43"/>
-      <c r="I40" s="44"/>
-      <c r="J40" s="44"/>
+      <c r="H40" s="35"/>
+      <c r="I40" s="36"/>
+      <c r="J40" s="36"/>
     </row>
   </sheetData>
   <mergeCells count="33">
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6382,6 +6365,23 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
26.10.19 Today Sales Update
</commit_message>
<xml_diff>
--- a/October/Others/Cash.xlsx
+++ b/October/Others/Cash.xlsx
@@ -107,7 +107,7 @@
     <t xml:space="preserve">                                                                          </t>
   </si>
   <si>
-    <t>Date: 21.10.19</t>
+    <t>Date: 26.10.19</t>
   </si>
 </sst>
 </file>
@@ -494,12 +494,39 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -509,32 +536,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -551,49 +564,36 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -601,12 +601,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -628,6 +622,12 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2076,7 +2076,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2098,60 +2098,60 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
@@ -2160,10 +2160,10 @@
       <c r="D5" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="14" t="s">
         <v>5</v>
       </c>
@@ -2178,10 +2178,10 @@
       <c r="D6" s="13">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>50</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="13">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>50000</v>
@@ -2197,10 +2197,10 @@
       <c r="D7" s="13">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>16</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="13">
         <f t="shared" si="0"/>
         <v>8000</v>
@@ -2216,10 +2216,10 @@
       <c r="D8" s="13">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>151</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="13">
         <f t="shared" si="0"/>
         <v>15100</v>
@@ -2235,10 +2235,10 @@
       <c r="D9" s="13">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>58</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="13">
         <f t="shared" si="0"/>
         <v>2900</v>
@@ -2254,8 +2254,8 @@
       <c r="D10" s="13">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2271,8 +2271,8 @@
       <c r="D11" s="13">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -2285,10 +2285,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14">
         <f>SUM(G6:G11)</f>
@@ -2335,58 +2335,58 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -2396,11 +2396,11 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -2475,60 +2475,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>16</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="24.95" customHeight="1">
       <c r="A31" s="6"/>
@@ -2537,10 +2537,10 @@
       <c r="D31" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="15" t="s">
         <v>5</v>
       </c>
@@ -2555,10 +2555,10 @@
       <c r="D32" s="16">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>50</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="16">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>50000</v>
@@ -2574,10 +2574,10 @@
       <c r="D33" s="16">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>116</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="16">
         <f t="shared" si="1"/>
         <v>58000</v>
@@ -2593,10 +2593,10 @@
       <c r="D34" s="16">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>151</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="16">
         <f t="shared" si="1"/>
         <v>15100</v>
@@ -2612,10 +2612,10 @@
       <c r="D35" s="16">
         <v>50</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>58</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="16">
         <f t="shared" si="1"/>
         <v>2900</v>
@@ -2631,8 +2631,8 @@
       <c r="D36" s="16">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="16">
         <f>SUM(D36*E36)</f>
         <v>0</v>
@@ -2648,8 +2648,8 @@
       <c r="D37" s="16">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="16">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -2662,10 +2662,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="37" t="s">
+      <c r="D38" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="38"/>
+      <c r="E38" s="47"/>
       <c r="F38" s="15"/>
       <c r="G38" s="15">
         <f>SUM(G32:G37)</f>
@@ -2712,58 +2712,58 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="6"/>
@@ -2773,11 +2773,11 @@
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -2805,6 +2805,32 @@
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -2817,32 +2843,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0.25" footer="0"/>
   <pageSetup scale="85" orientation="portrait" r:id="rId1"/>
@@ -2873,63 +2873,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="49" t="s">
+      <c r="A1" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="F1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="50" t="s">
+      <c r="A2" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="50"/>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="55"/>
+      <c r="D2" s="55"/>
+      <c r="E2" s="55"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="55"/>
+      <c r="I2" s="55"/>
+      <c r="J2" s="55"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="50" t="s">
+      <c r="A3" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="50"/>
-      <c r="C3" s="50"/>
-      <c r="D3" s="50"/>
-      <c r="E3" s="50"/>
-      <c r="F3" s="50"/>
-      <c r="G3" s="50"/>
-      <c r="H3" s="50"/>
-      <c r="I3" s="50"/>
-      <c r="J3" s="50"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="55"/>
+      <c r="D3" s="55"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="51" t="s">
+      <c r="A4" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B4" s="51"/>
-      <c r="C4" s="51"/>
-      <c r="D4" s="51"/>
-      <c r="E4" s="51"/>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="51"/>
-      <c r="J4" s="51"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
+      <c r="G4" s="56"/>
+      <c r="H4" s="56"/>
+      <c r="I4" s="56"/>
+      <c r="J4" s="56"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -2939,10 +2939,10 @@
       <c r="D5" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="52"/>
+      <c r="F5" s="57"/>
       <c r="G5" s="29" t="s">
         <v>5</v>
       </c>
@@ -2957,13 +2957,13 @@
       <c r="D6" s="24">
         <v>1000</v>
       </c>
-      <c r="E6" s="53">
-        <v>35</v>
-      </c>
-      <c r="F6" s="53"/>
+      <c r="E6" s="58">
+        <v>113</v>
+      </c>
+      <c r="F6" s="58"/>
       <c r="G6" s="24">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
-        <v>35000</v>
+        <v>113000</v>
       </c>
       <c r="H6" s="26"/>
       <c r="I6" s="26"/>
@@ -2976,13 +2976,13 @@
       <c r="D7" s="24">
         <v>500</v>
       </c>
-      <c r="E7" s="53">
-        <v>237</v>
-      </c>
-      <c r="F7" s="53"/>
+      <c r="E7" s="58">
+        <v>176</v>
+      </c>
+      <c r="F7" s="58"/>
       <c r="G7" s="24">
         <f t="shared" si="0"/>
-        <v>118500</v>
+        <v>88000</v>
       </c>
       <c r="H7" s="26"/>
       <c r="I7" s="26"/>
@@ -2995,13 +2995,13 @@
       <c r="D8" s="24">
         <v>100</v>
       </c>
-      <c r="E8" s="53">
-        <v>77</v>
-      </c>
-      <c r="F8" s="53"/>
+      <c r="E8" s="58">
+        <v>163</v>
+      </c>
+      <c r="F8" s="58"/>
       <c r="G8" s="24">
         <f t="shared" si="0"/>
-        <v>7700</v>
+        <v>16300</v>
       </c>
       <c r="H8" s="26"/>
       <c r="I8" s="26"/>
@@ -3014,13 +3014,13 @@
       <c r="D9" s="24">
         <v>50</v>
       </c>
-      <c r="E9" s="53">
-        <v>9</v>
-      </c>
-      <c r="F9" s="53"/>
+      <c r="E9" s="58">
+        <v>115</v>
+      </c>
+      <c r="F9" s="58"/>
       <c r="G9" s="24">
         <f t="shared" si="0"/>
-        <v>450</v>
+        <v>5750</v>
       </c>
       <c r="H9" s="26"/>
       <c r="I9" s="26"/>
@@ -3033,13 +3033,13 @@
       <c r="D10" s="24">
         <v>20</v>
       </c>
-      <c r="E10" s="53">
-        <v>14</v>
-      </c>
-      <c r="F10" s="53"/>
+      <c r="E10" s="58">
+        <v>37</v>
+      </c>
+      <c r="F10" s="58"/>
       <c r="G10" s="24">
         <f t="shared" si="0"/>
-        <v>280</v>
+        <v>740</v>
       </c>
       <c r="H10" s="26"/>
       <c r="I10" s="26"/>
@@ -3052,13 +3052,13 @@
       <c r="D11" s="24">
         <v>10</v>
       </c>
-      <c r="E11" s="53">
-        <v>107</v>
-      </c>
-      <c r="F11" s="53"/>
+      <c r="E11" s="58">
+        <v>21</v>
+      </c>
+      <c r="F11" s="58"/>
       <c r="G11" s="24">
         <f t="shared" si="0"/>
-        <v>1070</v>
+        <v>210</v>
       </c>
       <c r="H11" s="26"/>
       <c r="I11" s="26"/>
@@ -3068,14 +3068,14 @@
       <c r="A12" s="26"/>
       <c r="B12" s="26"/>
       <c r="C12" s="26"/>
-      <c r="D12" s="55" t="s">
+      <c r="D12" s="61" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="55"/>
+      <c r="E12" s="61"/>
       <c r="F12" s="25"/>
       <c r="G12" s="23">
         <f>SUM(G6:G11)</f>
-        <v>163000</v>
+        <v>224000</v>
       </c>
       <c r="H12" s="26"/>
       <c r="I12" s="26"/>
@@ -3127,35 +3127,35 @@
       <c r="E16" s="32"/>
       <c r="F16" s="30"/>
       <c r="G16" s="30"/>
-      <c r="H16" s="54" t="s">
+      <c r="H16" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I16" s="54"/>
-      <c r="J16" s="54"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="51"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="30"/>
-      <c r="D17" s="54"/>
+      <c r="D17" s="51"/>
       <c r="E17" s="30"/>
       <c r="F17" s="30"/>
       <c r="G17" s="30"/>
-      <c r="H17" s="54"/>
-      <c r="I17" s="54"/>
-      <c r="J17" s="54"/>
+      <c r="H17" s="51"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="51"/>
     </row>
     <row r="18" spans="1:10">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="30"/>
-      <c r="D18" s="54"/>
+      <c r="D18" s="51"/>
       <c r="E18" s="30"/>
       <c r="F18" s="30"/>
       <c r="G18" s="30"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
+      <c r="H18" s="51"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="51"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1" ht="17.25" customHeight="1">
       <c r="A19" s="32"/>
@@ -3167,9 +3167,9 @@
       <c r="E19" s="30"/>
       <c r="F19" s="30"/>
       <c r="G19" s="30"/>
-      <c r="H19" s="56"/>
-      <c r="I19" s="56"/>
-      <c r="J19" s="56"/>
+      <c r="H19" s="53"/>
+      <c r="I19" s="53"/>
+      <c r="J19" s="53"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="31"/>
@@ -3179,9 +3179,9 @@
       <c r="E20" s="31"/>
       <c r="F20" s="31"/>
       <c r="G20" s="31"/>
-      <c r="H20" s="57"/>
-      <c r="I20" s="58"/>
-      <c r="J20" s="58"/>
+      <c r="H20" s="49"/>
+      <c r="I20" s="50"/>
+      <c r="J20" s="50"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="31"/>
@@ -3268,60 +3268,60 @@
       <c r="J27" s="26"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="49" t="s">
+      <c r="A28" s="54" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="49"/>
-      <c r="E28" s="49"/>
-      <c r="F28" s="49"/>
-      <c r="G28" s="49"/>
-      <c r="H28" s="49"/>
-      <c r="I28" s="49"/>
-      <c r="J28" s="49"/>
+      <c r="B28" s="54"/>
+      <c r="C28" s="54"/>
+      <c r="D28" s="54"/>
+      <c r="E28" s="54"/>
+      <c r="F28" s="54"/>
+      <c r="G28" s="54"/>
+      <c r="H28" s="54"/>
+      <c r="I28" s="54"/>
+      <c r="J28" s="54"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="50" t="s">
+      <c r="A29" s="55" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="50"/>
-      <c r="C29" s="50"/>
-      <c r="D29" s="50"/>
-      <c r="E29" s="50"/>
-      <c r="F29" s="50"/>
-      <c r="G29" s="50"/>
-      <c r="H29" s="50"/>
-      <c r="I29" s="50"/>
-      <c r="J29" s="50"/>
+      <c r="B29" s="55"/>
+      <c r="C29" s="55"/>
+      <c r="D29" s="55"/>
+      <c r="E29" s="55"/>
+      <c r="F29" s="55"/>
+      <c r="G29" s="55"/>
+      <c r="H29" s="55"/>
+      <c r="I29" s="55"/>
+      <c r="J29" s="55"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="51" t="s">
+      <c r="A30" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="51"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
-      <c r="G30" s="51"/>
-      <c r="H30" s="51"/>
-      <c r="I30" s="51"/>
-      <c r="J30" s="51"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="56"/>
+      <c r="D30" s="56"/>
+      <c r="E30" s="56"/>
+      <c r="F30" s="56"/>
+      <c r="G30" s="56"/>
+      <c r="H30" s="56"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="56"/>
     </row>
     <row r="31" spans="1:10" ht="40.5" customHeight="1">
-      <c r="A31" s="51" t="s">
+      <c r="A31" s="56" t="s">
         <v>27</v>
       </c>
-      <c r="B31" s="51"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
-      <c r="G31" s="51"/>
-      <c r="H31" s="51"/>
-      <c r="I31" s="51"/>
-      <c r="J31" s="51"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="56"/>
+      <c r="D31" s="56"/>
+      <c r="E31" s="56"/>
+      <c r="F31" s="56"/>
+      <c r="G31" s="56"/>
+      <c r="H31" s="56"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
     </row>
     <row r="32" spans="1:10" ht="27.95" customHeight="1">
       <c r="A32" s="26"/>
@@ -3330,10 +3330,10 @@
       <c r="D32" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="52" t="s">
+      <c r="E32" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="52"/>
+      <c r="F32" s="57"/>
       <c r="G32" s="29" t="s">
         <v>5</v>
       </c>
@@ -3348,13 +3348,13 @@
       <c r="D33" s="21">
         <v>1000</v>
       </c>
-      <c r="E33" s="53">
-        <v>35</v>
-      </c>
-      <c r="F33" s="53"/>
+      <c r="E33" s="58">
+        <v>113</v>
+      </c>
+      <c r="F33" s="58"/>
       <c r="G33" s="21">
         <f t="shared" ref="G33:G38" si="1">SUM(D33*E33)</f>
-        <v>35000</v>
+        <v>113000</v>
       </c>
       <c r="H33" s="26"/>
       <c r="I33" s="26"/>
@@ -3367,13 +3367,13 @@
       <c r="D34" s="21">
         <v>500</v>
       </c>
-      <c r="E34" s="53">
-        <v>237</v>
-      </c>
-      <c r="F34" s="53"/>
+      <c r="E34" s="58">
+        <v>176</v>
+      </c>
+      <c r="F34" s="58"/>
       <c r="G34" s="21">
         <f t="shared" si="1"/>
-        <v>118500</v>
+        <v>88000</v>
       </c>
       <c r="H34" s="26"/>
       <c r="I34" s="26"/>
@@ -3386,13 +3386,13 @@
       <c r="D35" s="21">
         <v>100</v>
       </c>
-      <c r="E35" s="53">
-        <v>77</v>
-      </c>
-      <c r="F35" s="53"/>
+      <c r="E35" s="58">
+        <v>163</v>
+      </c>
+      <c r="F35" s="58"/>
       <c r="G35" s="21">
         <f t="shared" si="1"/>
-        <v>7700</v>
+        <v>16300</v>
       </c>
       <c r="H35" s="26"/>
       <c r="I35" s="26"/>
@@ -3405,13 +3405,13 @@
       <c r="D36" s="21">
         <v>50</v>
       </c>
-      <c r="E36" s="53">
-        <v>9</v>
-      </c>
-      <c r="F36" s="53"/>
+      <c r="E36" s="58">
+        <v>115</v>
+      </c>
+      <c r="F36" s="58"/>
       <c r="G36" s="21">
         <f t="shared" si="1"/>
-        <v>450</v>
+        <v>5750</v>
       </c>
       <c r="H36" s="26"/>
       <c r="I36" s="26"/>
@@ -3424,13 +3424,13 @@
       <c r="D37" s="21">
         <v>20</v>
       </c>
-      <c r="E37" s="53">
-        <v>14</v>
-      </c>
-      <c r="F37" s="53"/>
+      <c r="E37" s="58">
+        <v>37</v>
+      </c>
+      <c r="F37" s="58"/>
       <c r="G37" s="21">
         <f>SUM(D37*E37)</f>
-        <v>280</v>
+        <v>740</v>
       </c>
       <c r="H37" s="26"/>
       <c r="I37" s="26"/>
@@ -3443,13 +3443,13 @@
       <c r="D38" s="21">
         <v>10</v>
       </c>
-      <c r="E38" s="53">
-        <v>107</v>
-      </c>
-      <c r="F38" s="53"/>
+      <c r="E38" s="58">
+        <v>21</v>
+      </c>
+      <c r="F38" s="58"/>
       <c r="G38" s="21">
         <f t="shared" si="1"/>
-        <v>1070</v>
+        <v>210</v>
       </c>
       <c r="H38" s="26"/>
       <c r="I38" s="26"/>
@@ -3459,14 +3459,14 @@
       <c r="A39" s="26"/>
       <c r="B39" s="26"/>
       <c r="C39" s="26"/>
-      <c r="D39" s="60" t="s">
+      <c r="D39" s="59" t="s">
         <v>10</v>
       </c>
-      <c r="E39" s="61"/>
+      <c r="E39" s="60"/>
       <c r="F39" s="27"/>
       <c r="G39" s="22">
         <f>SUM(G33:G38)</f>
-        <v>163000</v>
+        <v>224000</v>
       </c>
       <c r="H39" s="26"/>
       <c r="I39" s="26"/>
@@ -3518,35 +3518,35 @@
       <c r="E43" s="28"/>
       <c r="F43" s="28"/>
       <c r="G43" s="28"/>
-      <c r="H43" s="54" t="s">
+      <c r="H43" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="I43" s="54"/>
-      <c r="J43" s="54"/>
+      <c r="I43" s="51"/>
+      <c r="J43" s="51"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="33"/>
       <c r="B44" s="33"/>
       <c r="C44" s="26"/>
-      <c r="D44" s="59"/>
+      <c r="D44" s="52"/>
       <c r="E44" s="26"/>
       <c r="F44" s="26"/>
       <c r="G44" s="26"/>
-      <c r="H44" s="59"/>
-      <c r="I44" s="59"/>
-      <c r="J44" s="59"/>
+      <c r="H44" s="52"/>
+      <c r="I44" s="52"/>
+      <c r="J44" s="52"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="33"/>
       <c r="B45" s="33"/>
       <c r="C45" s="26"/>
-      <c r="D45" s="59"/>
+      <c r="D45" s="52"/>
       <c r="E45" s="26"/>
       <c r="F45" s="26"/>
       <c r="G45" s="26"/>
-      <c r="H45" s="59"/>
-      <c r="I45" s="59"/>
-      <c r="J45" s="59"/>
+      <c r="H45" s="52"/>
+      <c r="I45" s="52"/>
+      <c r="J45" s="52"/>
     </row>
     <row r="46" spans="1:10" s="4" customFormat="1">
       <c r="A46" s="32"/>
@@ -3558,11 +3558,11 @@
       <c r="E46" s="28"/>
       <c r="F46" s="28"/>
       <c r="G46" s="28"/>
-      <c r="H46" s="56" t="s">
+      <c r="H46" s="53" t="s">
         <v>26</v>
       </c>
-      <c r="I46" s="56"/>
-      <c r="J46" s="56"/>
+      <c r="I46" s="53"/>
+      <c r="J46" s="53"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -3572,9 +3572,9 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="6"/>
@@ -3602,6 +3602,26 @@
     </row>
   </sheetData>
   <mergeCells count="34">
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="D17:D18"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E38:F38"/>
     <mergeCell ref="H47:J47"/>
     <mergeCell ref="H20:J20"/>
     <mergeCell ref="H43:J43"/>
@@ -3616,26 +3636,6 @@
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="D44:D45"/>
     <mergeCell ref="D39:E39"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="D17:D18"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
   </mergeCells>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup scale="75" orientation="portrait" r:id="rId1"/>
@@ -3666,63 +3666,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -3732,10 +3732,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -3750,10 +3750,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>68</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>68000</v>
@@ -3769,10 +3769,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>135</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>67500</v>
@@ -3788,10 +3788,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>53</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>5300</v>
@@ -3807,10 +3807,10 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41">
+      <c r="E9" s="39">
         <v>2</v>
       </c>
-      <c r="F9" s="41"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3826,10 +3826,10 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41">
+      <c r="E10" s="39">
         <v>5</v>
       </c>
-      <c r="F10" s="41"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>100</v>
@@ -3845,8 +3845,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -3859,10 +3859,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -3909,76 +3909,76 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40" t="s">
+      <c r="A19" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B19" s="40"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="62" t="s">
         <v>14</v>
       </c>
-      <c r="B20" s="63"/>
+      <c r="B20" s="62"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4053,60 +4053,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="20.25">
       <c r="A31" s="6"/>
@@ -4115,10 +4115,10 @@
       <c r="D31" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="62" t="s">
+      <c r="E31" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="62"/>
+      <c r="F31" s="66"/>
       <c r="G31" s="9" t="s">
         <v>5</v>
       </c>
@@ -4133,10 +4133,10 @@
       <c r="D32" s="2">
         <v>1000</v>
       </c>
-      <c r="E32" s="66">
+      <c r="E32" s="65">
         <v>68</v>
       </c>
-      <c r="F32" s="66"/>
+      <c r="F32" s="65"/>
       <c r="G32" s="2">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>68000</v>
@@ -4152,10 +4152,10 @@
       <c r="D33" s="2">
         <v>500</v>
       </c>
-      <c r="E33" s="66">
+      <c r="E33" s="65">
         <v>135</v>
       </c>
-      <c r="F33" s="66"/>
+      <c r="F33" s="65"/>
       <c r="G33" s="2">
         <f t="shared" si="1"/>
         <v>67500</v>
@@ -4171,10 +4171,10 @@
       <c r="D34" s="2">
         <v>100</v>
       </c>
-      <c r="E34" s="66">
+      <c r="E34" s="65">
         <v>53</v>
       </c>
-      <c r="F34" s="66"/>
+      <c r="F34" s="65"/>
       <c r="G34" s="2">
         <f t="shared" si="1"/>
         <v>5300</v>
@@ -4190,10 +4190,10 @@
       <c r="D35" s="2">
         <v>50</v>
       </c>
-      <c r="E35" s="66">
+      <c r="E35" s="65">
         <v>2</v>
       </c>
-      <c r="F35" s="66"/>
+      <c r="F35" s="65"/>
       <c r="G35" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4209,10 +4209,10 @@
       <c r="D36" s="2">
         <v>20</v>
       </c>
-      <c r="E36" s="66">
+      <c r="E36" s="65">
         <v>5</v>
       </c>
-      <c r="F36" s="66"/>
+      <c r="F36" s="65"/>
       <c r="G36" s="2">
         <f t="shared" si="1"/>
         <v>100</v>
@@ -4228,8 +4228,8 @@
       <c r="D37" s="2">
         <v>10</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="2">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4242,10 +4242,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="65" t="s">
+      <c r="D38" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="65"/>
+      <c r="E38" s="64"/>
       <c r="F38" s="9"/>
       <c r="G38" s="9">
         <f>SUM(G32:G37)</f>
@@ -4292,76 +4292,76 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40" t="s">
+      <c r="A45" s="41" t="s">
         <v>13</v>
       </c>
-      <c r="B45" s="40"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64" t="s">
+      <c r="A46" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="B46" s="64"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -4389,6 +4389,30 @@
     </row>
   </sheetData>
   <mergeCells count="40">
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A27:J27"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
     <mergeCell ref="H46:J46"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="A46:B46"/>
@@ -4405,30 +4429,6 @@
     <mergeCell ref="E35:F35"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A27:J27"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -4460,63 +4460,63 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
       <c r="K1" s="1"/>
     </row>
     <row r="2" spans="1:11" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="18">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="37" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
       <c r="K3" s="1"/>
     </row>
     <row r="4" spans="1:11" ht="42" customHeight="1">
-      <c r="A4" s="45" t="s">
+      <c r="A4" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
       <c r="K4" s="1"/>
     </row>
     <row r="5" spans="1:11" ht="27.95" customHeight="1">
@@ -4526,10 +4526,10 @@
       <c r="D5" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="E5" s="46" t="s">
+      <c r="E5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F5" s="46"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="8" t="s">
         <v>5</v>
       </c>
@@ -4544,10 +4544,10 @@
       <c r="D6" s="3">
         <v>1000</v>
       </c>
-      <c r="E6" s="41">
+      <c r="E6" s="39">
         <v>44</v>
       </c>
-      <c r="F6" s="41"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="3">
         <f t="shared" ref="G6:G11" si="0">SUM(D6*E6)</f>
         <v>44000</v>
@@ -4563,10 +4563,10 @@
       <c r="D7" s="3">
         <v>500</v>
       </c>
-      <c r="E7" s="41">
+      <c r="E7" s="39">
         <v>118</v>
       </c>
-      <c r="F7" s="41"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="3">
         <f t="shared" si="0"/>
         <v>59000</v>
@@ -4582,10 +4582,10 @@
       <c r="D8" s="3">
         <v>100</v>
       </c>
-      <c r="E8" s="41">
+      <c r="E8" s="39">
         <v>510</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="3">
         <f t="shared" si="0"/>
         <v>51000</v>
@@ -4601,8 +4601,8 @@
       <c r="D9" s="3">
         <v>50</v>
       </c>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4618,8 +4618,8 @@
       <c r="D10" s="3">
         <v>20</v>
       </c>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4635,8 +4635,8 @@
       <c r="D11" s="3">
         <v>10</v>
       </c>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -4649,10 +4649,10 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="E12" s="46"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="8"/>
       <c r="G12" s="8">
         <f>SUM(G6:G11)</f>
@@ -4699,72 +4699,72 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:11">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="47"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47" t="s">
+      <c r="H16" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10" s="4" customFormat="1">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48" t="s">
+      <c r="H19" s="42" t="s">
         <v>12</v>
       </c>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
-      <c r="A20" s="67"/>
-      <c r="B20" s="67"/>
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35" t="s">
+      <c r="H20" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -4839,60 +4839,60 @@
       <c r="J26" s="6"/>
     </row>
     <row r="27" spans="1:10" ht="31.5">
-      <c r="A27" s="42" t="s">
+      <c r="A27" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B27" s="42"/>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
-      <c r="G27" s="42"/>
-      <c r="H27" s="42"/>
-      <c r="I27" s="42"/>
-      <c r="J27" s="42"/>
+      <c r="B27" s="36"/>
+      <c r="C27" s="36"/>
+      <c r="D27" s="36"/>
+      <c r="E27" s="36"/>
+      <c r="F27" s="36"/>
+      <c r="G27" s="36"/>
+      <c r="H27" s="36"/>
+      <c r="I27" s="36"/>
+      <c r="J27" s="36"/>
     </row>
     <row r="28" spans="1:10" ht="18">
-      <c r="A28" s="43" t="s">
+      <c r="A28" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B28" s="43"/>
-      <c r="C28" s="43"/>
-      <c r="D28" s="43"/>
-      <c r="E28" s="43"/>
-      <c r="F28" s="43"/>
-      <c r="G28" s="43"/>
-      <c r="H28" s="43"/>
-      <c r="I28" s="43"/>
-      <c r="J28" s="43"/>
+      <c r="B28" s="37"/>
+      <c r="C28" s="37"/>
+      <c r="D28" s="37"/>
+      <c r="E28" s="37"/>
+      <c r="F28" s="37"/>
+      <c r="G28" s="37"/>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
+      <c r="J28" s="37"/>
     </row>
     <row r="29" spans="1:10" ht="18.75">
-      <c r="A29" s="44" t="s">
+      <c r="A29" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B29" s="44"/>
-      <c r="C29" s="44"/>
-      <c r="D29" s="44"/>
-      <c r="E29" s="44"/>
-      <c r="F29" s="44"/>
-      <c r="G29" s="44"/>
-      <c r="H29" s="44"/>
-      <c r="I29" s="44"/>
-      <c r="J29" s="44"/>
+      <c r="B29" s="45"/>
+      <c r="C29" s="45"/>
+      <c r="D29" s="45"/>
+      <c r="E29" s="45"/>
+      <c r="F29" s="45"/>
+      <c r="G29" s="45"/>
+      <c r="H29" s="45"/>
+      <c r="I29" s="45"/>
+      <c r="J29" s="45"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="45" t="s">
+      <c r="A30" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B30" s="45"/>
-      <c r="C30" s="45"/>
-      <c r="D30" s="45"/>
-      <c r="E30" s="45"/>
-      <c r="F30" s="45"/>
-      <c r="G30" s="45"/>
-      <c r="H30" s="45"/>
-      <c r="I30" s="45"/>
-      <c r="J30" s="45"/>
+      <c r="B30" s="38"/>
+      <c r="C30" s="38"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="38"/>
+      <c r="F30" s="38"/>
+      <c r="G30" s="38"/>
+      <c r="H30" s="38"/>
+      <c r="I30" s="38"/>
+      <c r="J30" s="38"/>
     </row>
     <row r="31" spans="1:10" ht="23.25">
       <c r="A31" s="6"/>
@@ -4901,10 +4901,10 @@
       <c r="D31" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E31" s="46" t="s">
+      <c r="E31" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="F31" s="46"/>
+      <c r="F31" s="35"/>
       <c r="G31" s="12" t="s">
         <v>5</v>
       </c>
@@ -4919,10 +4919,10 @@
       <c r="D32" s="11">
         <v>1000</v>
       </c>
-      <c r="E32" s="41">
+      <c r="E32" s="39">
         <v>44</v>
       </c>
-      <c r="F32" s="41"/>
+      <c r="F32" s="39"/>
       <c r="G32" s="11">
         <f t="shared" ref="G32:G37" si="1">SUM(D32*E32)</f>
         <v>44000</v>
@@ -4938,10 +4938,10 @@
       <c r="D33" s="11">
         <v>500</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>118</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="11">
         <f t="shared" si="1"/>
         <v>59000</v>
@@ -4957,10 +4957,10 @@
       <c r="D34" s="11">
         <v>100</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>510</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="11">
         <f t="shared" si="1"/>
         <v>51000</v>
@@ -4976,8 +4976,8 @@
       <c r="D35" s="11">
         <v>50</v>
       </c>
-      <c r="E35" s="41"/>
-      <c r="F35" s="41"/>
+      <c r="E35" s="39"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -4993,8 +4993,8 @@
       <c r="D36" s="11">
         <v>20</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5010,8 +5010,8 @@
       <c r="D37" s="11">
         <v>10</v>
       </c>
-      <c r="E37" s="41"/>
-      <c r="F37" s="41"/>
+      <c r="E37" s="39"/>
+      <c r="F37" s="39"/>
       <c r="G37" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
@@ -5024,10 +5024,10 @@
       <c r="A38" s="6"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="68" t="s">
+      <c r="D38" s="67" t="s">
         <v>10</v>
       </c>
-      <c r="E38" s="68"/>
+      <c r="E38" s="67"/>
       <c r="F38" s="12"/>
       <c r="G38" s="12">
         <f>SUM(G32:G37)</f>
@@ -5074,72 +5074,72 @@
       <c r="J41" s="6"/>
     </row>
     <row r="42" spans="1:10" s="5" customFormat="1" ht="15.75">
-      <c r="A42" s="39" t="s">
+      <c r="A42" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B42" s="39"/>
+      <c r="B42" s="48"/>
       <c r="C42" s="7"/>
       <c r="D42" s="7"/>
       <c r="E42" s="7"/>
       <c r="F42" s="7"/>
       <c r="G42" s="7"/>
-      <c r="H42" s="39" t="s">
+      <c r="H42" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I42" s="39"/>
-      <c r="J42" s="39"/>
+      <c r="I42" s="48"/>
+      <c r="J42" s="48"/>
     </row>
     <row r="43" spans="1:10">
-      <c r="A43" s="40"/>
-      <c r="B43" s="40"/>
+      <c r="A43" s="41"/>
+      <c r="B43" s="41"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
       <c r="E43" s="6"/>
       <c r="F43" s="6"/>
       <c r="G43" s="6"/>
-      <c r="H43" s="40"/>
-      <c r="I43" s="40"/>
-      <c r="J43" s="40"/>
+      <c r="H43" s="41"/>
+      <c r="I43" s="41"/>
+      <c r="J43" s="41"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10" s="4" customFormat="1" ht="15.75">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40" t="s">
+      <c r="H45" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I45" s="39"/>
-      <c r="J45" s="39"/>
+      <c r="I45" s="48"/>
+      <c r="J45" s="48"/>
     </row>
     <row r="46" spans="1:10">
-      <c r="A46" s="64"/>
-      <c r="B46" s="64"/>
+      <c r="A46" s="63"/>
+      <c r="B46" s="63"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="35" t="s">
+      <c r="H46" s="43" t="s">
         <v>11</v>
       </c>
-      <c r="I46" s="36"/>
-      <c r="J46" s="36"/>
+      <c r="I46" s="44"/>
+      <c r="J46" s="44"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5167,16 +5167,24 @@
     </row>
   </sheetData>
   <mergeCells count="40">
-    <mergeCell ref="A45:B45"/>
-    <mergeCell ref="H45:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="D38:E38"/>
-    <mergeCell ref="A42:B42"/>
-    <mergeCell ref="H42:J42"/>
-    <mergeCell ref="A43:B44"/>
-    <mergeCell ref="H43:J44"/>
+    <mergeCell ref="D12:E12"/>
+    <mergeCell ref="A1:J1"/>
+    <mergeCell ref="A2:J2"/>
+    <mergeCell ref="A3:J3"/>
+    <mergeCell ref="A4:J4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E7:F7"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="E9:F9"/>
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="A20:B20"/>
     <mergeCell ref="H20:J20"/>
@@ -5189,24 +5197,16 @@
     <mergeCell ref="E33:F33"/>
     <mergeCell ref="E34:F34"/>
     <mergeCell ref="E35:F35"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="D12:E12"/>
-    <mergeCell ref="A1:J1"/>
-    <mergeCell ref="A2:J2"/>
-    <mergeCell ref="A3:J3"/>
-    <mergeCell ref="A4:J4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E7:F7"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="E9:F9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="A45:B45"/>
+    <mergeCell ref="H45:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="D38:E38"/>
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="H42:J42"/>
+    <mergeCell ref="A43:B44"/>
+    <mergeCell ref="H43:J44"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.5" right="0" top="0" bottom="0" header="0" footer="0"/>
@@ -5231,64 +5231,64 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="3" spans="1:10" ht="18">
-      <c r="A3" s="43"/>
-      <c r="B3" s="43"/>
-      <c r="C3" s="43"/>
-      <c r="D3" s="43"/>
-      <c r="E3" s="43"/>
-      <c r="F3" s="43"/>
-      <c r="G3" s="43"/>
-      <c r="H3" s="43"/>
-      <c r="I3" s="43"/>
-      <c r="J3" s="43"/>
+      <c r="A3" s="37"/>
+      <c r="B3" s="37"/>
+      <c r="C3" s="37"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="37"/>
+      <c r="F3" s="37"/>
+      <c r="G3" s="37"/>
+      <c r="H3" s="37"/>
+      <c r="I3" s="37"/>
+      <c r="J3" s="37"/>
     </row>
     <row r="4" spans="1:10" ht="18.75">
-      <c r="A4" s="45"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="45"/>
-      <c r="D4" s="45"/>
-      <c r="E4" s="45"/>
-      <c r="F4" s="45"/>
-      <c r="G4" s="45"/>
-      <c r="H4" s="45"/>
-      <c r="I4" s="45"/>
-      <c r="J4" s="45"/>
+      <c r="A4" s="38"/>
+      <c r="B4" s="38"/>
+      <c r="C4" s="38"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="38"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="38"/>
+      <c r="J4" s="38"/>
     </row>
     <row r="5" spans="1:10" ht="23.25">
       <c r="A5" s="6"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
       <c r="D5" s="18"/>
-      <c r="E5" s="46"/>
-      <c r="F5" s="46"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
       <c r="G5" s="18"/>
       <c r="H5" s="6"/>
       <c r="I5" s="6"/>
@@ -5299,8 +5299,8 @@
       <c r="B6" s="6"/>
       <c r="C6" s="6"/>
       <c r="D6" s="17"/>
-      <c r="E6" s="41"/>
-      <c r="F6" s="41"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
       <c r="G6" s="17"/>
       <c r="H6" s="6"/>
       <c r="I6" s="6"/>
@@ -5311,8 +5311,8 @@
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
       <c r="D7" s="17"/>
-      <c r="E7" s="41"/>
-      <c r="F7" s="41"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
       <c r="G7" s="17"/>
       <c r="H7" s="6"/>
       <c r="I7" s="6"/>
@@ -5323,8 +5323,8 @@
       <c r="B8" s="6"/>
       <c r="C8" s="6"/>
       <c r="D8" s="17"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="E8" s="39"/>
+      <c r="F8" s="39"/>
       <c r="G8" s="17"/>
       <c r="H8" s="6"/>
       <c r="I8" s="6"/>
@@ -5335,8 +5335,8 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
       <c r="D9" s="17"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9" s="17"/>
       <c r="H9" s="6"/>
       <c r="I9" s="6"/>
@@ -5347,8 +5347,8 @@
       <c r="B10" s="6"/>
       <c r="C10" s="6"/>
       <c r="D10" s="17"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+      <c r="E10" s="39"/>
+      <c r="F10" s="39"/>
       <c r="G10" s="17"/>
       <c r="H10" s="6"/>
       <c r="I10" s="6"/>
@@ -5359,8 +5359,8 @@
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
       <c r="D11" s="17"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+      <c r="E11" s="39"/>
+      <c r="F11" s="39"/>
       <c r="G11" s="17"/>
       <c r="H11" s="6"/>
       <c r="I11" s="6"/>
@@ -5370,8 +5370,8 @@
       <c r="A12" s="6"/>
       <c r="B12" s="6"/>
       <c r="C12" s="6"/>
-      <c r="D12" s="46"/>
-      <c r="E12" s="46"/>
+      <c r="D12" s="35"/>
+      <c r="E12" s="35"/>
       <c r="F12" s="18"/>
       <c r="G12" s="18"/>
       <c r="H12" s="6"/>
@@ -5415,52 +5415,52 @@
       <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10">
-      <c r="A16" s="47"/>
-      <c r="B16" s="47"/>
+      <c r="A16" s="40"/>
+      <c r="B16" s="40"/>
       <c r="C16" s="10"/>
       <c r="D16" s="10"/>
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="47"/>
-      <c r="I16" s="47"/>
-      <c r="J16" s="47"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="40"/>
+      <c r="J16" s="40"/>
     </row>
     <row r="17" spans="1:10">
-      <c r="A17" s="47"/>
-      <c r="B17" s="47"/>
+      <c r="A17" s="40"/>
+      <c r="B17" s="40"/>
       <c r="C17" s="10"/>
       <c r="D17" s="10"/>
       <c r="E17" s="10"/>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
-      <c r="H17" s="47"/>
-      <c r="I17" s="47"/>
-      <c r="J17" s="47"/>
+      <c r="H17" s="40"/>
+      <c r="I17" s="40"/>
+      <c r="J17" s="40"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="47"/>
-      <c r="B18" s="47"/>
+      <c r="A18" s="40"/>
+      <c r="B18" s="40"/>
       <c r="C18" s="10"/>
       <c r="D18" s="10"/>
       <c r="E18" s="10"/>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
-      <c r="H18" s="47"/>
-      <c r="I18" s="47"/>
-      <c r="J18" s="47"/>
+      <c r="H18" s="40"/>
+      <c r="I18" s="40"/>
+      <c r="J18" s="40"/>
     </row>
     <row r="19" spans="1:10">
-      <c r="A19" s="40"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="41"/>
+      <c r="B19" s="41"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
       <c r="F19" s="6"/>
       <c r="G19" s="6"/>
-      <c r="H19" s="48"/>
-      <c r="I19" s="48"/>
-      <c r="J19" s="48"/>
+      <c r="H19" s="42"/>
+      <c r="I19" s="42"/>
+      <c r="J19" s="42"/>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="6"/>
@@ -5470,9 +5470,9 @@
       <c r="E20" s="6"/>
       <c r="F20" s="6"/>
       <c r="G20" s="6"/>
-      <c r="H20" s="35"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="44"/>
+      <c r="J20" s="44"/>
     </row>
     <row r="21" spans="1:10">
       <c r="A21" s="6"/>
@@ -5559,60 +5559,60 @@
       <c r="J27" s="6"/>
     </row>
     <row r="28" spans="1:10" ht="31.5">
-      <c r="A28" s="42" t="s">
+      <c r="A28" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B28" s="42"/>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
-      <c r="G28" s="42"/>
-      <c r="H28" s="42"/>
-      <c r="I28" s="42"/>
-      <c r="J28" s="42"/>
+      <c r="B28" s="36"/>
+      <c r="C28" s="36"/>
+      <c r="D28" s="36"/>
+      <c r="E28" s="36"/>
+      <c r="F28" s="36"/>
+      <c r="G28" s="36"/>
+      <c r="H28" s="36"/>
+      <c r="I28" s="36"/>
+      <c r="J28" s="36"/>
     </row>
     <row r="29" spans="1:10" ht="18">
-      <c r="A29" s="43" t="s">
+      <c r="A29" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B29" s="43"/>
-      <c r="C29" s="43"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="43"/>
-      <c r="F29" s="43"/>
-      <c r="G29" s="43"/>
-      <c r="H29" s="43"/>
-      <c r="I29" s="43"/>
-      <c r="J29" s="43"/>
+      <c r="B29" s="37"/>
+      <c r="C29" s="37"/>
+      <c r="D29" s="37"/>
+      <c r="E29" s="37"/>
+      <c r="F29" s="37"/>
+      <c r="G29" s="37"/>
+      <c r="H29" s="37"/>
+      <c r="I29" s="37"/>
+      <c r="J29" s="37"/>
     </row>
     <row r="30" spans="1:10" ht="18.75">
-      <c r="A30" s="44" t="s">
+      <c r="A30" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B30" s="44"/>
-      <c r="C30" s="44"/>
-      <c r="D30" s="44"/>
-      <c r="E30" s="44"/>
-      <c r="F30" s="44"/>
-      <c r="G30" s="44"/>
-      <c r="H30" s="44"/>
-      <c r="I30" s="44"/>
-      <c r="J30" s="44"/>
+      <c r="B30" s="45"/>
+      <c r="C30" s="45"/>
+      <c r="D30" s="45"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
+      <c r="G30" s="45"/>
+      <c r="H30" s="45"/>
+      <c r="I30" s="45"/>
+      <c r="J30" s="45"/>
     </row>
     <row r="31" spans="1:10" ht="18.75">
-      <c r="A31" s="45" t="s">
+      <c r="A31" s="38" t="s">
         <v>19</v>
       </c>
-      <c r="B31" s="45"/>
-      <c r="C31" s="45"/>
-      <c r="D31" s="45"/>
-      <c r="E31" s="45"/>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45"/>
-      <c r="H31" s="45"/>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
+      <c r="B31" s="38"/>
+      <c r="C31" s="38"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="38"/>
+      <c r="F31" s="38"/>
+      <c r="G31" s="38"/>
+      <c r="H31" s="38"/>
+      <c r="I31" s="38"/>
+      <c r="J31" s="38"/>
     </row>
     <row r="32" spans="1:10" ht="20.25">
       <c r="A32" s="6" t="s">
@@ -5623,10 +5623,10 @@
       <c r="D32" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E32" s="62" t="s">
+      <c r="E32" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F32" s="62"/>
+      <c r="F32" s="66"/>
       <c r="G32" s="20" t="s">
         <v>5</v>
       </c>
@@ -5641,10 +5641,10 @@
       <c r="D33" s="19">
         <v>1000</v>
       </c>
-      <c r="E33" s="41">
+      <c r="E33" s="39">
         <v>30</v>
       </c>
-      <c r="F33" s="41"/>
+      <c r="F33" s="39"/>
       <c r="G33" s="19">
         <f t="shared" ref="G33:G38" si="0">SUM(D33*E33)</f>
         <v>30000</v>
@@ -5660,10 +5660,10 @@
       <c r="D34" s="19">
         <v>500</v>
       </c>
-      <c r="E34" s="41">
+      <c r="E34" s="39">
         <v>35</v>
       </c>
-      <c r="F34" s="41"/>
+      <c r="F34" s="39"/>
       <c r="G34" s="19">
         <f t="shared" si="0"/>
         <v>17500</v>
@@ -5679,10 +5679,10 @@
       <c r="D35" s="19">
         <v>100</v>
       </c>
-      <c r="E35" s="41">
+      <c r="E35" s="39">
         <v>425</v>
       </c>
-      <c r="F35" s="41"/>
+      <c r="F35" s="39"/>
       <c r="G35" s="19">
         <f t="shared" si="0"/>
         <v>42500</v>
@@ -5698,8 +5698,8 @@
       <c r="D36" s="19">
         <v>50</v>
       </c>
-      <c r="E36" s="41"/>
-      <c r="F36" s="41"/>
+      <c r="E36" s="39"/>
+      <c r="F36" s="39"/>
       <c r="G36" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -5715,8 +5715,8 @@
       <c r="D37" s="19">
         <v>20</v>
       </c>
-      <c r="E37" s="66"/>
-      <c r="F37" s="66"/>
+      <c r="E37" s="65"/>
+      <c r="F37" s="65"/>
       <c r="G37" s="19">
         <f>SUM(D37*E37)</f>
         <v>0</v>
@@ -5732,10 +5732,10 @@
       <c r="D38" s="19">
         <v>10</v>
       </c>
-      <c r="E38" s="66">
+      <c r="E38" s="65">
         <v>100</v>
       </c>
-      <c r="F38" s="66"/>
+      <c r="F38" s="65"/>
       <c r="G38" s="19">
         <f t="shared" si="0"/>
         <v>1000</v>
@@ -5798,58 +5798,58 @@
       <c r="J42" s="6"/>
     </row>
     <row r="43" spans="1:10" ht="15.75">
-      <c r="A43" s="39" t="s">
+      <c r="A43" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B43" s="39"/>
+      <c r="B43" s="48"/>
       <c r="C43" s="7"/>
       <c r="D43" s="7"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
       <c r="G43" s="7"/>
-      <c r="H43" s="39" t="s">
+      <c r="H43" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I43" s="39"/>
-      <c r="J43" s="39"/>
+      <c r="I43" s="48"/>
+      <c r="J43" s="48"/>
     </row>
     <row r="44" spans="1:10">
-      <c r="A44" s="40"/>
-      <c r="B44" s="40"/>
+      <c r="A44" s="41"/>
+      <c r="B44" s="41"/>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
       <c r="F44" s="6"/>
       <c r="G44" s="6"/>
-      <c r="H44" s="40"/>
-      <c r="I44" s="40"/>
-      <c r="J44" s="40"/>
+      <c r="H44" s="41"/>
+      <c r="I44" s="41"/>
+      <c r="J44" s="41"/>
     </row>
     <row r="45" spans="1:10">
-      <c r="A45" s="40"/>
-      <c r="B45" s="40"/>
+      <c r="A45" s="41"/>
+      <c r="B45" s="41"/>
       <c r="C45" s="6"/>
       <c r="D45" s="6"/>
       <c r="E45" s="6"/>
       <c r="F45" s="6"/>
       <c r="G45" s="6"/>
-      <c r="H45" s="40"/>
-      <c r="I45" s="40"/>
-      <c r="J45" s="40"/>
+      <c r="H45" s="41"/>
+      <c r="I45" s="41"/>
+      <c r="J45" s="41"/>
     </row>
     <row r="46" spans="1:10" ht="15.75">
-      <c r="A46" s="40"/>
-      <c r="B46" s="40"/>
+      <c r="A46" s="41"/>
+      <c r="B46" s="41"/>
       <c r="C46" s="6"/>
       <c r="D46" s="6"/>
       <c r="E46" s="6"/>
       <c r="F46" s="6"/>
       <c r="G46" s="6"/>
-      <c r="H46" s="40" t="s">
+      <c r="H46" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="39"/>
-      <c r="J46" s="39"/>
+      <c r="I46" s="48"/>
+      <c r="J46" s="48"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="6"/>
@@ -5859,12 +5859,38 @@
       <c r="E47" s="6"/>
       <c r="F47" s="6"/>
       <c r="G47" s="6"/>
-      <c r="H47" s="35"/>
-      <c r="I47" s="36"/>
-      <c r="J47" s="36"/>
+      <c r="H47" s="43"/>
+      <c r="I47" s="44"/>
+      <c r="J47" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="38">
+    <mergeCell ref="H47:J47"/>
+    <mergeCell ref="D39:E39"/>
+    <mergeCell ref="A43:B43"/>
+    <mergeCell ref="H43:J43"/>
+    <mergeCell ref="A44:B45"/>
+    <mergeCell ref="H44:J45"/>
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="H46:J46"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="H20:J20"/>
+    <mergeCell ref="A28:J28"/>
+    <mergeCell ref="A29:J29"/>
+    <mergeCell ref="A30:J30"/>
+    <mergeCell ref="A31:J31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="E33:F33"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="E36:F36"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="A17:B18"/>
+    <mergeCell ref="H17:J18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="H19:J19"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
@@ -5877,32 +5903,6 @@
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="E10:F10"/>
     <mergeCell ref="E11:F11"/>
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="A17:B18"/>
-    <mergeCell ref="H17:J18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="H19:J19"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="H20:J20"/>
-    <mergeCell ref="A28:J28"/>
-    <mergeCell ref="A29:J29"/>
-    <mergeCell ref="A30:J30"/>
-    <mergeCell ref="A31:J31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="E33:F33"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="E36:F36"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="H47:J47"/>
-    <mergeCell ref="D39:E39"/>
-    <mergeCell ref="A43:B43"/>
-    <mergeCell ref="H43:J43"/>
-    <mergeCell ref="A44:B45"/>
-    <mergeCell ref="H44:J45"/>
-    <mergeCell ref="A46:B46"/>
-    <mergeCell ref="H46:J46"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -5928,177 +5928,177 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" ht="31.5">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
-      <c r="H1" s="42"/>
-      <c r="I1" s="42"/>
-      <c r="J1" s="42"/>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
     </row>
     <row r="2" spans="1:10" ht="18">
-      <c r="A2" s="43" t="s">
+      <c r="A2" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="43"/>
-      <c r="C2" s="43"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="43"/>
-      <c r="F2" s="43"/>
-      <c r="G2" s="43"/>
-      <c r="H2" s="43"/>
-      <c r="I2" s="43"/>
-      <c r="J2" s="43"/>
+      <c r="B2" s="37"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="37"/>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="80">
+      <c r="A5" s="79">
         <v>1</v>
       </c>
-      <c r="B5" s="73" t="s">
+      <c r="B5" s="71" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="71">
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="78">
         <v>1650</v>
       </c>
     </row>
     <row r="6" spans="1:10">
-      <c r="A6" s="80"/>
-      <c r="B6" s="73"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="71"/>
+      <c r="A6" s="79"/>
+      <c r="B6" s="71"/>
+      <c r="C6" s="71"/>
+      <c r="D6" s="71"/>
+      <c r="E6" s="71"/>
+      <c r="F6" s="71"/>
+      <c r="G6" s="78"/>
     </row>
     <row r="7" spans="1:10">
-      <c r="A7" s="80">
+      <c r="A7" s="79">
         <v>2</v>
       </c>
-      <c r="B7" s="73" t="s">
+      <c r="B7" s="71" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="73"/>
-      <c r="D7" s="73"/>
-      <c r="E7" s="73"/>
-      <c r="F7" s="73"/>
-      <c r="G7" s="71">
+      <c r="C7" s="71"/>
+      <c r="D7" s="71"/>
+      <c r="E7" s="71"/>
+      <c r="F7" s="71"/>
+      <c r="G7" s="78">
         <v>1980</v>
       </c>
     </row>
     <row r="8" spans="1:10">
-      <c r="A8" s="80"/>
-      <c r="B8" s="73"/>
-      <c r="C8" s="73"/>
-      <c r="D8" s="73"/>
-      <c r="E8" s="73"/>
-      <c r="F8" s="73"/>
-      <c r="G8" s="71"/>
+      <c r="A8" s="79"/>
+      <c r="B8" s="71"/>
+      <c r="C8" s="71"/>
+      <c r="D8" s="71"/>
+      <c r="E8" s="71"/>
+      <c r="F8" s="71"/>
+      <c r="G8" s="78"/>
     </row>
     <row r="9" spans="1:10">
-      <c r="A9" s="80">
+      <c r="A9" s="79">
         <v>3</v>
       </c>
-      <c r="B9" s="73" t="s">
+      <c r="B9" s="71" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="73"/>
-      <c r="D9" s="73"/>
-      <c r="E9" s="73"/>
-      <c r="F9" s="73"/>
-      <c r="G9" s="71">
+      <c r="C9" s="71"/>
+      <c r="D9" s="71"/>
+      <c r="E9" s="71"/>
+      <c r="F9" s="71"/>
+      <c r="G9" s="78">
         <v>10538</v>
       </c>
     </row>
     <row r="10" spans="1:10">
-      <c r="A10" s="80"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="73"/>
-      <c r="D10" s="73"/>
-      <c r="E10" s="73"/>
-      <c r="F10" s="73"/>
-      <c r="G10" s="71"/>
+      <c r="A10" s="79"/>
+      <c r="B10" s="71"/>
+      <c r="C10" s="71"/>
+      <c r="D10" s="71"/>
+      <c r="E10" s="71"/>
+      <c r="F10" s="71"/>
+      <c r="G10" s="78"/>
     </row>
     <row r="11" spans="1:10">
-      <c r="A11" s="80">
+      <c r="A11" s="79">
         <v>4</v>
       </c>
-      <c r="B11" s="74" t="s">
+      <c r="B11" s="72" t="s">
         <v>23</v>
       </c>
-      <c r="C11" s="75"/>
-      <c r="D11" s="75"/>
-      <c r="E11" s="75"/>
-      <c r="F11" s="76"/>
-      <c r="G11" s="71">
+      <c r="C11" s="73"/>
+      <c r="D11" s="73"/>
+      <c r="E11" s="73"/>
+      <c r="F11" s="74"/>
+      <c r="G11" s="78">
         <v>1100</v>
       </c>
     </row>
     <row r="12" spans="1:10">
-      <c r="A12" s="80"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="79"/>
-      <c r="G12" s="71"/>
+      <c r="A12" s="79"/>
+      <c r="B12" s="75"/>
+      <c r="C12" s="76"/>
+      <c r="D12" s="76"/>
+      <c r="E12" s="76"/>
+      <c r="F12" s="77"/>
+      <c r="G12" s="78"/>
     </row>
     <row r="13" spans="1:10">
-      <c r="A13" s="72" t="s">
+      <c r="A13" s="80" t="s">
         <v>24</v>
       </c>
-      <c r="B13" s="72"/>
-      <c r="C13" s="72"/>
-      <c r="D13" s="72"/>
-      <c r="E13" s="72"/>
-      <c r="F13" s="72"/>
-      <c r="G13" s="71">
+      <c r="B13" s="80"/>
+      <c r="C13" s="80"/>
+      <c r="D13" s="80"/>
+      <c r="E13" s="80"/>
+      <c r="F13" s="80"/>
+      <c r="G13" s="78">
         <f>SUM(G5:G12)</f>
         <v>15268</v>
       </c>
     </row>
     <row r="14" spans="1:10">
-      <c r="A14" s="72"/>
-      <c r="B14" s="72"/>
-      <c r="C14" s="72"/>
-      <c r="D14" s="72"/>
-      <c r="E14" s="72"/>
-      <c r="F14" s="72"/>
-      <c r="G14" s="71"/>
+      <c r="A14" s="80"/>
+      <c r="B14" s="80"/>
+      <c r="C14" s="80"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="80"/>
+      <c r="F14" s="80"/>
+      <c r="G14" s="78"/>
     </row>
     <row r="23" spans="1:10" ht="18.75">
-      <c r="A23" s="44" t="s">
+      <c r="A23" s="45" t="s">
         <v>9</v>
       </c>
-      <c r="B23" s="44"/>
-      <c r="C23" s="44"/>
-      <c r="D23" s="44"/>
-      <c r="E23" s="44"/>
-      <c r="F23" s="44"/>
-      <c r="G23" s="44"/>
-      <c r="H23" s="44"/>
-      <c r="I23" s="44"/>
-      <c r="J23" s="44"/>
+      <c r="B23" s="45"/>
+      <c r="C23" s="45"/>
+      <c r="D23" s="45"/>
+      <c r="E23" s="45"/>
+      <c r="F23" s="45"/>
+      <c r="G23" s="45"/>
+      <c r="H23" s="45"/>
+      <c r="I23" s="45"/>
+      <c r="J23" s="45"/>
     </row>
     <row r="24" spans="1:10" ht="18.75">
-      <c r="A24" s="45"/>
-      <c r="B24" s="45"/>
-      <c r="C24" s="45"/>
-      <c r="D24" s="45"/>
-      <c r="E24" s="45"/>
-      <c r="F24" s="45"/>
-      <c r="G24" s="45"/>
-      <c r="H24" s="45"/>
-      <c r="I24" s="45"/>
-      <c r="J24" s="45"/>
+      <c r="A24" s="38"/>
+      <c r="B24" s="38"/>
+      <c r="C24" s="38"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="38"/>
+      <c r="F24" s="38"/>
+      <c r="G24" s="38"/>
+      <c r="H24" s="38"/>
+      <c r="I24" s="38"/>
+      <c r="J24" s="38"/>
     </row>
     <row r="25" spans="1:10" ht="20.25">
       <c r="A25" s="6" t="s">
@@ -6109,10 +6109,10 @@
       <c r="D25" s="20" t="s">
         <v>3</v>
       </c>
-      <c r="E25" s="62" t="s">
+      <c r="E25" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F25" s="62"/>
+      <c r="F25" s="66"/>
       <c r="G25" s="20" t="s">
         <v>5</v>
       </c>
@@ -6127,8 +6127,8 @@
       <c r="D26" s="19">
         <v>1000</v>
       </c>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="E26" s="39"/>
+      <c r="F26" s="39"/>
       <c r="G26" s="19">
         <f t="shared" ref="G26:G31" si="0">SUM(D26*E26)</f>
         <v>0</v>
@@ -6144,10 +6144,10 @@
       <c r="D27" s="19">
         <v>500</v>
       </c>
-      <c r="E27" s="41">
+      <c r="E27" s="39">
         <v>30</v>
       </c>
-      <c r="F27" s="41"/>
+      <c r="F27" s="39"/>
       <c r="G27" s="19">
         <f t="shared" si="0"/>
         <v>15000</v>
@@ -6163,8 +6163,8 @@
       <c r="D28" s="19">
         <v>100</v>
       </c>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="E28" s="39"/>
+      <c r="F28" s="39"/>
       <c r="G28" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
@@ -6180,10 +6180,10 @@
       <c r="D29" s="19">
         <v>50</v>
       </c>
-      <c r="E29" s="41">
+      <c r="E29" s="39">
         <v>5</v>
       </c>
-      <c r="F29" s="41"/>
+      <c r="F29" s="39"/>
       <c r="G29" s="19">
         <f t="shared" si="0"/>
         <v>250</v>
@@ -6199,8 +6199,8 @@
       <c r="D30" s="19">
         <v>20</v>
       </c>
-      <c r="E30" s="66"/>
-      <c r="F30" s="66"/>
+      <c r="E30" s="65"/>
+      <c r="F30" s="65"/>
       <c r="G30" s="19">
         <f>SUM(D30*E30)</f>
         <v>0</v>
@@ -6216,10 +6216,10 @@
       <c r="D31" s="19">
         <v>10</v>
       </c>
-      <c r="E31" s="66">
+      <c r="E31" s="65">
         <v>2</v>
       </c>
-      <c r="F31" s="66"/>
+      <c r="F31" s="65"/>
       <c r="G31" s="19">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -6282,58 +6282,58 @@
       <c r="J35" s="6"/>
     </row>
     <row r="36" spans="1:10" ht="15.75">
-      <c r="A36" s="39" t="s">
+      <c r="A36" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="B36" s="39"/>
+      <c r="B36" s="48"/>
       <c r="C36" s="7"/>
       <c r="D36" s="7"/>
       <c r="E36" s="7"/>
       <c r="F36" s="7"/>
       <c r="G36" s="7"/>
-      <c r="H36" s="39" t="s">
+      <c r="H36" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="48"/>
+      <c r="J36" s="48"/>
     </row>
     <row r="37" spans="1:10">
-      <c r="A37" s="40"/>
-      <c r="B37" s="40"/>
+      <c r="A37" s="41"/>
+      <c r="B37" s="41"/>
       <c r="C37" s="6"/>
       <c r="D37" s="6"/>
       <c r="E37" s="6"/>
       <c r="F37" s="6"/>
       <c r="G37" s="6"/>
-      <c r="H37" s="40"/>
-      <c r="I37" s="40"/>
-      <c r="J37" s="40"/>
+      <c r="H37" s="41"/>
+      <c r="I37" s="41"/>
+      <c r="J37" s="41"/>
     </row>
     <row r="38" spans="1:10">
-      <c r="A38" s="40"/>
-      <c r="B38" s="40"/>
+      <c r="A38" s="41"/>
+      <c r="B38" s="41"/>
       <c r="C38" s="6"/>
       <c r="D38" s="6"/>
       <c r="E38" s="6"/>
       <c r="F38" s="6"/>
       <c r="G38" s="6"/>
-      <c r="H38" s="40"/>
-      <c r="I38" s="40"/>
-      <c r="J38" s="40"/>
+      <c r="H38" s="41"/>
+      <c r="I38" s="41"/>
+      <c r="J38" s="41"/>
     </row>
     <row r="39" spans="1:10" ht="15.75">
-      <c r="A39" s="40"/>
-      <c r="B39" s="40"/>
+      <c r="A39" s="41"/>
+      <c r="B39" s="41"/>
       <c r="C39" s="6"/>
       <c r="D39" s="6"/>
       <c r="E39" s="6"/>
       <c r="F39" s="6"/>
       <c r="G39" s="6"/>
-      <c r="H39" s="40" t="s">
+      <c r="H39" s="41" t="s">
         <v>12</v>
       </c>
-      <c r="I39" s="39"/>
-      <c r="J39" s="39"/>
+      <c r="I39" s="48"/>
+      <c r="J39" s="48"/>
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="6"/>
@@ -6343,12 +6343,29 @@
       <c r="E40" s="6"/>
       <c r="F40" s="6"/>
       <c r="G40" s="6"/>
-      <c r="H40" s="35"/>
-      <c r="I40" s="36"/>
-      <c r="J40" s="36"/>
+      <c r="H40" s="43"/>
+      <c r="I40" s="44"/>
+      <c r="J40" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="H40:J40"/>
+    <mergeCell ref="D32:E32"/>
+    <mergeCell ref="A36:B36"/>
+    <mergeCell ref="H36:J36"/>
+    <mergeCell ref="A37:B38"/>
+    <mergeCell ref="H37:J38"/>
+    <mergeCell ref="A39:B39"/>
+    <mergeCell ref="H39:J39"/>
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="A13:F14"/>
+    <mergeCell ref="E31:F31"/>
+    <mergeCell ref="G13:G14"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E30:F30"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A2:J2"/>
     <mergeCell ref="A23:J23"/>
@@ -6365,23 +6382,6 @@
     <mergeCell ref="B5:F6"/>
     <mergeCell ref="G5:G6"/>
     <mergeCell ref="B7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="A13:F14"/>
-    <mergeCell ref="E31:F31"/>
-    <mergeCell ref="G13:G14"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="H40:J40"/>
-    <mergeCell ref="D32:E32"/>
-    <mergeCell ref="A36:B36"/>
-    <mergeCell ref="H36:J36"/>
-    <mergeCell ref="A37:B38"/>
-    <mergeCell ref="H37:J38"/>
-    <mergeCell ref="A39:B39"/>
-    <mergeCell ref="H39:J39"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="71" orientation="portrait" r:id="rId1"/>

</xml_diff>